<commit_message>
Aggiunte nuove analisi e tracciamento tempi di valutazione perr CodeGen
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/AnalisiCodeGen.xlsx
+++ b/HE/W_in_progress/AnalisiCodeGen.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28209"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F3F549F-800E-472A-BD97-64CADD984DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8AA68D5-BF92-4DC9-8954-CA6483AFA676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="866">
   <si>
     <t>IN</t>
   </si>
@@ -1800,6 +1800,9 @@
     <t>process(clk) begin if rising_edge(clk) then if counter = DIV - 1 then pwm_out &lt;= '1'; else pwm_out &lt;= '0'; end if; counter &lt;= counter + 1; end if; end process;</t>
   </si>
   <si>
+    <t>Credo sia un codice equivalente</t>
+  </si>
+  <si>
     <t>Generate a CRC checker of N-bit with the signals data_in (N-bit), received_CRC (M-bit), and polynomial (M-bit) as input and the signal CRC_match as output.</t>
   </si>
   <si>
@@ -1809,6 +1812,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity crc_checker is Generic (N : natural := 8; M : natural := 16); Port ( Data_In : in STD_LOGIC_VECTOR (N-1 downto 0); Received_CRC : in STD_LOGIC_VECTOR (M-1 downto 0); Polynomial : in STD_LOGIC_VECTOR (M-1 downto 0); CRC_Match : out STD_LOGIC); end crc_checker; architecture Behavioral of crc_checker is begin process (Data_In, Received_CRC, Polynomial) variable received_crc : STD_LOGIC_VECTOR (M-1 downto 0); variable polynomial : STD_LOGIC_VECTOR (M-1 downto 0); begin received_crc := Data_In; polynomial := Polynomial; for i in 0 to N-1 loop if received_crc(M-1) = '1' then received_crc := received_crc(M-2 downto 0) &amp; '0'; else received_crc := received_crc(M-1 downto 1) &amp; '0'; end if ; end loop ; CRC_Match &lt;= '1' when (received_crc = Polynomial) else '0'; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Codice equivalente</t>
+  </si>
+  <si>
     <t>Define a fixed-point divider of N-bit with the signals dividend (N-bit) and divisor (N-bit) as input and the signals quotient (N-bit) and remainder (N-bit) as output.</t>
   </si>
   <si>
@@ -1827,6 +1833,27 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity magnitude_comparator is Port ( A1 : in STD_LOGIC; A0 : in STD_LOGIC; B1 : in STD_LOGIC; B0 : in STD_LOGIC; A_greater : out STD_LOGIC; A_equal : out STD_LOGIC; A_smaller : out STD_LOGIC); end magnitude_comparator; architecture Behavioral of magnitude_comparator is begin process (A1, A0, B1, B0) variable a, b: integer range 0 to 3; begin a := 0; b := 0; if (A1 = '1') then a := 1; elsif (A1 = '0') then a := 0; elsif (A1 = '+') then a := 1; elsif (A1 = '-'') then a := 0; elsif (A1 = '+' and A2 = '0') then a := 1; elsif (A1 = '-' and A2 = '0') then a := 0; else a := 1; end if ; if (A2 = '1') then b := 1; elsif (A2 = '0') then b := 0; elsif (A2 = '+') then b := 1; elsif (A2 = '-') then b := 0; else b := 1; end if ; if (b = a) then A_greater &lt;= '1'; A_equal &lt;= '0'; A_Smaller &lt;= '0'; elsif (b = a) then A_Greater &lt;= '1'; A_Equal &lt;= '0'; A_Smaller &lt;= '0'; else A_Greater &lt;= '0'; A_E</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Contiene errori logici e sintattici </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>elsif (A1 = '+')</t>
+    </r>
+  </si>
+  <si>
     <t>Write a binary to gray converter of N-bit with the signal binary (N-bit) as input and the signal gray_code (N-bit) as output.</t>
   </si>
   <si>
@@ -1836,6 +1863,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity B2GConverter is Generic ( N : natural := 8 ); Port ( Binary : in STD_LOGIC_VECTOR (N-1 downto 0); Gray_Code : out STD_LOGIC_VECTOR (N-1 downto 0)); end B2GConverter; architecture Behavioral of B2GConverter is begin process (Binary) variable Gray_Code_temp : STD_LOGIC_VECTOR (N-1 downto 0); begin for i in 0 to N-1 loop if Binary(i) = '1' then Gray_Code_temp(i) := '0'; else Gray_Code_temp(i) := '1'; end if ; end loop ; Gray_Code &lt;= Gray_Code_temp; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t xml:space="preserve">Non implementa il convertitore ma il complemento a due </t>
+  </si>
+  <si>
     <t>Implement a basic quadrature encoder interface</t>
   </si>
   <si>
@@ -1845,6 +1875,9 @@
     <t>process(clk) begin if rising_edge(clk) then a_prev &lt;= a; b_prev &lt;= b; if a /= a_prev then if b /= a then count &lt;= count + 1; else count &lt;= count - 1; end if; end if; end if; end process;</t>
   </si>
   <si>
+    <t>Diversa logica ma dovrebbe essere un QEI</t>
+  </si>
+  <si>
     <t>Define a debouncer with the signal noisy_button as input and the signal clean_button_pulse as output.</t>
   </si>
   <si>
@@ -1854,6 +1887,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity debouncer is Port ( Noisy_Button : in STD_LOGIC; Clean_Button_Pulse : out STD_LOGIC); end debouncer; architecture Behavioral of debouncer is begin process (Noisy_Button) variable counter : integer range 0 to 10 := 0; begin if (Noisy_Button = '1') then counter := counter + 1; if (counter &gt;= 5) then Clean_Button_Pulse &lt;= '1'; else Clean_Button_Pulse &lt;= '0'; end if ; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Tutti e due implementano il debouncer</t>
+  </si>
+  <si>
     <t>Define a Johnson ring counter of N-bit with the signals clock and reset as input and the signal count (N-bit) as output.</t>
   </si>
   <si>
@@ -1872,6 +1908,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity pulse_generator is Port ( Clk : in STD_LOGIC; Reset : in STD_LOGIC; Pulse_Width : in STD_LOGIC_VECTOR (N-1 downto 0); Pulse_Out : out STD_LOGIC); end pulse_generator; architecture Behavioral of pulse_generator is signal count: unsigned(Pulse_Width) := (others =&gt; '0'); begin process (Clk, Reset) begin if Reset = '1' then count &lt;= (others =&gt; '0'); elsif rising_edge(Clk) then count &lt;= count + 1; end if ; end process ; Pulse_Out &lt;= '1' when count = Pulse_Width else '0'; end Behavioral;</t>
   </si>
   <si>
+    <t>Non implementa un pulse generator circuit</t>
+  </si>
+  <si>
     <t>Define a magnitude comparator of K-bit with the signals A (K-bit) and B (K-bit) as input and the signals A_GT_B, A_EQ_B, and A_LT_B as output.</t>
   </si>
   <si>
@@ -1881,6 +1920,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity magnitude_comparator is Generic ( K : natural := 8 ); Port ( A : in STD_LOGIC_VECTOR (K-1 downto 0); B : in STD_LOGIC_VECTOR (K-1 downto 0); A_GT_B : out STD_LOGIC; A_EQ_B : out STD_LOGIC; A_LT_B : out STD_LOGIC); end magnitude_comparator; architecture Behavioral of magnitude_comparator is begin process (A, B) variable a, b : integer range 0 to K-1; begin a := 0; b := 0; for i in 0 to K-1 loop if A(i) &gt; B(i) then a := i; b := i; end if ; end loop ; A_GT_B &lt;= a &gt; b; A_EQ_B &lt;= a = b; A_LT_B &lt;= a &lt; b; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t xml:space="preserve">Equivalenti, con logica diversa </t>
+  </si>
+  <si>
     <t>Define a pseudo-random number generator of N-bit with the signals clock and seed_value (N-bit) as input and the signal random_number (N-bit) as output.</t>
   </si>
   <si>
@@ -1890,6 +1932,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity PRNG is Generic(N : integer := 8); Port(Clock : in std_logic; Seed_Value : in std_logic_vector(N-1 downto 0); Random_Number : out std_logic_vector(N-1 downto 0)); end PRNG; architecture Behavioral of PRNG is begin process (Clock) variable seed : std_logic_vector(N-1 downto 0); variable random_number : std_logic_vector(N-1 downto 0); begin if (rising_edge(Clock)) then random_number := seed; for i in 0 to N-1 loop random_number(i) := random_number(i) xor random_number(i-1); end loop ; seed := random_number; end if ; end process ; Random_Number &lt;= random_number; end Behavioral;</t>
   </si>
   <si>
+    <t>La logica è diversa, forse questa meno corretta, ma implementano un codice di generazione pseudo-casuale dei numeri</t>
+  </si>
+  <si>
     <t>Create a configurable clock divider</t>
   </si>
   <si>
@@ -1899,6 +1944,9 @@
     <t>process(clk,rst)begin if rst='1'then clk_div&lt;=0;counter&lt;=0;elsif rising_edge(clk)then if counter=divisore_frequenza.duration then clk_div&lt;=1;counter&lt;=0;else clk_div&lt;=0;counter&lt;=counter+1;end if;end if;end process;</t>
   </si>
   <si>
+    <t>Logiche diverse ma sempre un divisore</t>
+  </si>
+  <si>
     <t>Write an astable multivibrator with the signals clk and reset as input and the signal oscillating_out as output.</t>
   </si>
   <si>
@@ -1908,6 +1956,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity AstableMultivibrator is Port ( Clk : in STD_LOGIC; Reset : in STD_LOGIC; Oscillating_Out : out STD_LOGIC); end AstableMultivibrator; architecture Behavioral of AstableMultivibrator is signal Counter : unsigned(31 downto 0) := (others =&gt; '0'); begin process (Clk, Reset) begin if Reset = '1' then Counter &lt;= (others =&gt; '0'); elsif rising_edge(Clk) then Counter &lt;= Counter + 1; end if ; end process ; Oscillating_Out &lt;= '1' when Counter = unsigned(31) else '0'; end Behavioral;</t>
   </si>
   <si>
+    <t>Tutti e due multivibratori astabili</t>
+  </si>
+  <si>
     <t>Define a rotating priority encoder with the signal request (N-bit) as input and the signals grant (log2N-bit), valid, and rotation_bit as output.</t>
   </si>
   <si>
@@ -1917,6 +1968,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity PriorityEncoder is Generic(N : integer := 8); Port ( Request : in STD_LOGIC_VECTOR (N-1 downto 0); Grant : out STD_LOGIC_VECTOR (log2(N)-1 downto 0); Valid : out STD_LOGIC; Rotation_Bit : out STD_LOGIC); end PriorityEncoder; architecture Behavioral of PriorityEncoder is begin process (Request) variable temp : STD_LOGIC_VECTOR (N-1 downto 0); begin temp := Request; for i in 0 to N-1 loop if temp(i) = '1' then Valid &lt;= '1'; Rotation_Bit &lt;= '0'; elsif Valid = '0' then Valid &lt;= '0'; Rotation_Bit &lt;= '1'; else Valid &lt;= '0'; Rotation_Bit &lt;= '0'; end if ; end loop ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non implementa un encode correttamente</t>
+  </si>
+  <si>
     <t>Generate a floating-point adder of N-bit with the signals A (N-bit) and B (N-bit) as input and the signal sum (N-bit) as output.</t>
   </si>
   <si>
@@ -1935,6 +1989,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity Digital_Comparator is Port ( A1 : in STD_LOGIC; A0 : in STD_LOGIC; B1 : in STD_LOGIC; B0 : in STD_LOGIC; A_GT_B : out STD_LOGIC; A_EQ_B : out STD_LOGIC; A_LT_B : out STD_LOGIC); end Digital_Comparator; architecture Behavioral of Digital_Comparator is begin process (A1, A0, B1, B0) variable a: std_logic_vector(3 downto 0); variable b: std_logic_vector(3 downto 0); begin a := (A1 &amp; A0) | (B1 &amp; B0); b := (A1 &amp; A0) | (B1 &amp; B0); if (a &gt; b) then A_GT_B &lt;= '1'; A_EQ_B &lt;= '0'; A_LT_B &lt;= '0'; elsif (a = b) then A_GT_B &lt;= '0'; A_EQ_B &lt;= '1'; A_LT_B &lt;= '0'; else A_GT_B &lt;= '0'; A_EQ_B &lt;= '0'; A_LT_B &lt;= '1'; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t xml:space="preserve">Contiene errori logici e sintattici </t>
+  </si>
+  <si>
     <t>Define a 2-to-1 multiplexer with the signals data0, data1, and select as input and the signal data_out as output.</t>
   </si>
   <si>
@@ -1950,6 +2007,9 @@
     <t>process(clk,rst)begin if rst='1'then sclk&lt;='0';mosi&lt;='0';cs&lt;='1';shift_reg&lt;=(others=&gt;'0');elsif rising_edge(clk)then cs&lt;='0';sclk&lt;=not sclk;if sclk='0'then shift_reg&lt;=shift_reg(6 downto 0)&amp;miso;mosi&lt;=shift_reg(7);if bit_count=7 then cs&lt;='1';end if;end if;end if;end process;</t>
   </si>
   <si>
+    <t>Due protocolli diversi</t>
+  </si>
+  <si>
     <t>Detect falling edge of a signal using a process.</t>
   </si>
   <si>
@@ -1959,6 +2019,9 @@
     <t>signal prev_signal: std_logic:='0';process(clk,rst)begin if rst='1'then prev_signal&lt;='0';elsif rising_edge(clk)then prev_signal&lt;=signal;end if;end process;</t>
   </si>
   <si>
+    <t>Lo do buono anche se non c'è output e non c'è reset</t>
+  </si>
+  <si>
     <t>Define a universal shift register of P-bit with the signals clock, shift_enable, shift_direction, and serial_in as input and the signals parallel_out (P-bit) and serial_out as output.</t>
   </si>
   <si>
@@ -1968,6 +2031,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity UniversalShiftRegister is Generic ( P : natural := 8 ); Port ( Clock : in STD_LOGIC; ShiftEnable : in STD_LOGIC; ShiftDirection : in STD_LOGIC; SerialIn : in STD_LOGIC_VECTOR (P-1 downto 0); ParallelOut : out STD_LOGIC_VECTOR (P-1 downto 0); SerialOut : out STD_LOGIC); end UniversalShiftRegister; architecture Behavioral of UniversalShiftRegister is signal shiftReg : STD_LOGIC_VECTOR(P-1 downto 0); begin process (Clock, ShiftEnable, ShiftDirection, SerialIn) begin if rising_edge(Clock) then if ShiftEnable = '1' then if ShiftDirection = '0' then shiftReg &lt;= shiftReg(P-2 downto 0) &amp; SerialIn; else shiftReg &lt;= shiftReg(P-1 downto 1) &amp; SerialIn; end if ; end if ; end if ; end process ; ParallelOut &lt;= shiftReg; SerialOut &lt;= shiftReg(P-1 downto 0); end Behavioral;</t>
   </si>
   <si>
+    <t>Non funziona lo shift a destra</t>
+  </si>
+  <si>
     <t>Implement a basic priority encoder</t>
   </si>
   <si>
@@ -1995,6 +2061,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity BinaryToBCDConverter is Generic ( N : natural := 8; M : natural := 3 ); Port ( Binary_Value : in STD_LOGIC_VECTOR (N-1 downto 0); BCD_Value : out STD_LOGIC_VECTOR ((M/3)+1-1 downto 0)); end BinaryToBCDConverter; architecture Behavioral of BinaryToBCDConverter is begin process (Binary_Value) variable temp : STD_LOGIC_VECTOR (N-1 downto 0); begin for i in 0 to N-1 loop temp(i) := Binary_Value(i); end loop ; BCD_Value &lt;= temp; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non implementa la logica BCD</t>
+  </si>
+  <si>
     <t>Create a pulse generator that outputs a single pulse every N clock cycles</t>
   </si>
   <si>
@@ -2004,6 +2073,9 @@
     <t>process(clk) begin if rising_edge(clk) then if counter = N - 1 then counter &lt;= 0; pulse &lt;= '1'; elsif counter = N - 2 then counter &lt;= 0; pulse &lt;= '0'; else counter &lt;= counter + 1; pulse &lt;= '1'; end if; end if; end process;</t>
   </si>
   <si>
+    <t>Va migliorato però grossomodo genera quello che ho chiesto</t>
+  </si>
+  <si>
     <t>Define a binary to BCD converter of (N/3)+1-digit with the signal binary_value (N-bit) as input and the signal BCD_value ((N/3)+1-digit) as output.</t>
   </si>
   <si>
@@ -2011,6 +2083,9 @@
   </si>
   <si>
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity BinaryToBCDConverter is Generic (N : integer := 8); Port ( Binary_Value : in STD_LOGIC_VECTOR (N-1 downto 0); BCD_Value : out STD_LOGIC_VECTOR ((N/3)+1-1 downto 0)); end BinaryToBCDConverter; architecture Behavioral of BinaryToBCDConverter is begin process (Binary_Value) variable temp : STD_LOGIC_VECTOR (N-1 downto 0); begin for i in 0 to N-1 loop temp(i) := Binary_Value(i); end loop ; BCD_Value &lt;= temp; end process ; end Behavioral;</t>
+  </si>
+  <si>
+    <t>Non corretto</t>
   </si>
   <si>
     <t>Define a dual-port RAM of K x L with the signals clock, write_enable, read_enable, write_address (log2K-bit), read_address (log2K-bit), and data_in (L-bit) as input and the signal data_out (L-bit) as output.</t>
@@ -2578,7 +2653,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2593,6 +2668,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -2634,12 +2715,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2944,8 +3026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
-      <selection activeCell="G236" sqref="G236"/>
+    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="G261" sqref="G261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8478,18 +8560,21 @@
         <v>0.70188492063492058</v>
       </c>
       <c r="G236">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H236" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="237" spans="1:8">
       <c r="A237" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B237" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C237" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D237">
         <v>0</v>
@@ -8501,18 +8586,21 @@
         <v>0.62499124171466203</v>
       </c>
       <c r="G237">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H237" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="238" spans="1:8">
       <c r="A238" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="B238" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="C238" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="D238">
         <v>0</v>
@@ -8524,18 +8612,21 @@
         <v>0.61077903654581056</v>
       </c>
       <c r="G238">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H238" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="239" spans="1:8">
       <c r="A239" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="B239" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="C239" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D239">
         <v>0</v>
@@ -8549,16 +8640,19 @@
       <c r="G239">
         <v>0</v>
       </c>
+      <c r="H239" s="3" t="s">
+        <v>600</v>
+      </c>
     </row>
     <row r="240" spans="1:8">
       <c r="A240" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="B240" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="C240" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="D240">
         <v>0</v>
@@ -8572,16 +8666,19 @@
       <c r="G240">
         <v>0</v>
       </c>
-    </row>
-    <row r="241" spans="1:7">
+      <c r="H240" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8">
       <c r="A241" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="B241" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
       <c r="C241" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="D241">
         <v>0</v>
@@ -8593,18 +8690,21 @@
         <v>0.31288072588951238</v>
       </c>
       <c r="G241">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="242" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H241" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8">
       <c r="A242" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="B242" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="C242" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
       <c r="D242">
         <v>0</v>
@@ -8616,18 +8716,21 @@
         <v>0.49607158826516312</v>
       </c>
       <c r="G242">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="243" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H242" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8">
       <c r="A243" t="s">
-        <v>607</v>
+        <v>613</v>
       </c>
       <c r="B243" t="s">
-        <v>608</v>
+        <v>614</v>
       </c>
       <c r="C243" t="s">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="D243">
         <v>0</v>
@@ -8639,18 +8742,18 @@
         <v>0.8377679543852905</v>
       </c>
       <c r="G243">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8">
       <c r="A244" t="s">
-        <v>610</v>
+        <v>616</v>
       </c>
       <c r="B244" t="s">
-        <v>611</v>
+        <v>617</v>
       </c>
       <c r="C244" t="s">
-        <v>612</v>
+        <v>618</v>
       </c>
       <c r="D244">
         <v>0</v>
@@ -8664,16 +8767,19 @@
       <c r="G244">
         <v>0</v>
       </c>
-    </row>
-    <row r="245" spans="1:7">
+      <c r="H244" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8">
       <c r="A245" t="s">
-        <v>613</v>
+        <v>620</v>
       </c>
       <c r="B245" t="s">
-        <v>614</v>
+        <v>621</v>
       </c>
       <c r="C245" t="s">
-        <v>615</v>
+        <v>622</v>
       </c>
       <c r="D245">
         <v>0</v>
@@ -8685,18 +8791,21 @@
         <v>0.57943898965099838</v>
       </c>
       <c r="G245">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="246" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H245" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8">
       <c r="A246" t="s">
-        <v>616</v>
+        <v>624</v>
       </c>
       <c r="B246" t="s">
-        <v>617</v>
+        <v>625</v>
       </c>
       <c r="C246" t="s">
-        <v>618</v>
+        <v>626</v>
       </c>
       <c r="D246">
         <v>0</v>
@@ -8708,18 +8817,21 @@
         <v>0.60428249294544478</v>
       </c>
       <c r="G246">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="247" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H246" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8">
       <c r="A247" t="s">
-        <v>619</v>
+        <v>628</v>
       </c>
       <c r="B247" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="C247" t="s">
-        <v>621</v>
+        <v>630</v>
       </c>
       <c r="D247">
         <v>0</v>
@@ -8731,18 +8843,21 @@
         <v>0.65513154380341887</v>
       </c>
       <c r="G247">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="248" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H247" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8">
       <c r="A248" t="s">
-        <v>622</v>
+        <v>632</v>
       </c>
       <c r="B248" t="s">
-        <v>623</v>
+        <v>633</v>
       </c>
       <c r="C248" t="s">
-        <v>624</v>
+        <v>634</v>
       </c>
       <c r="D248">
         <v>0</v>
@@ -8754,18 +8869,21 @@
         <v>0.76545995282535129</v>
       </c>
       <c r="G248">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="249" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H248" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8">
       <c r="A249" t="s">
-        <v>625</v>
+        <v>636</v>
       </c>
       <c r="B249" t="s">
-        <v>626</v>
+        <v>637</v>
       </c>
       <c r="C249" t="s">
-        <v>627</v>
+        <v>638</v>
       </c>
       <c r="D249">
         <v>0</v>
@@ -8779,16 +8897,19 @@
       <c r="G249">
         <v>0</v>
       </c>
-    </row>
-    <row r="250" spans="1:7">
+      <c r="H249" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8">
       <c r="A250" t="s">
-        <v>628</v>
+        <v>640</v>
       </c>
       <c r="B250" t="s">
-        <v>629</v>
+        <v>641</v>
       </c>
       <c r="C250" t="s">
-        <v>630</v>
+        <v>642</v>
       </c>
       <c r="D250">
         <v>0</v>
@@ -8800,18 +8921,18 @@
         <v>0.59366365984966929</v>
       </c>
       <c r="G250">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="251" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8">
       <c r="A251" t="s">
-        <v>631</v>
+        <v>643</v>
       </c>
       <c r="B251" t="s">
-        <v>632</v>
+        <v>644</v>
       </c>
       <c r="C251" t="s">
-        <v>633</v>
+        <v>645</v>
       </c>
       <c r="D251">
         <v>0</v>
@@ -8825,16 +8946,19 @@
       <c r="G251">
         <v>0</v>
       </c>
-    </row>
-    <row r="252" spans="1:7">
+      <c r="H251" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8">
       <c r="A252" t="s">
-        <v>634</v>
+        <v>647</v>
       </c>
       <c r="B252" t="s">
-        <v>635</v>
+        <v>648</v>
       </c>
       <c r="C252" t="s">
-        <v>636</v>
+        <v>649</v>
       </c>
       <c r="D252">
         <v>0</v>
@@ -8846,15 +8970,15 @@
         <v>0.71172702986774106</v>
       </c>
       <c r="G252">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="253" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8">
       <c r="A253" t="s">
-        <v>637</v>
+        <v>650</v>
       </c>
       <c r="B253" t="s">
-        <v>638</v>
+        <v>651</v>
       </c>
       <c r="C253" t="s">
         <v>560</v>
@@ -8871,16 +8995,19 @@
       <c r="G253">
         <v>0</v>
       </c>
-    </row>
-    <row r="254" spans="1:7">
+      <c r="H253" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8">
       <c r="A254" t="s">
-        <v>639</v>
+        <v>653</v>
       </c>
       <c r="B254" t="s">
-        <v>640</v>
+        <v>654</v>
       </c>
       <c r="C254" t="s">
-        <v>641</v>
+        <v>655</v>
       </c>
       <c r="D254">
         <v>0</v>
@@ -8892,18 +9019,21 @@
         <v>0.86962368001147439</v>
       </c>
       <c r="G254">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="255" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H254" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8">
       <c r="A255" t="s">
-        <v>642</v>
+        <v>657</v>
       </c>
       <c r="B255" t="s">
-        <v>643</v>
+        <v>658</v>
       </c>
       <c r="C255" t="s">
-        <v>644</v>
+        <v>659</v>
       </c>
       <c r="D255">
         <v>0</v>
@@ -8917,16 +9047,19 @@
       <c r="G255">
         <v>0</v>
       </c>
-    </row>
-    <row r="256" spans="1:7">
+      <c r="H255" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8">
       <c r="A256" t="s">
-        <v>645</v>
+        <v>661</v>
       </c>
       <c r="B256" t="s">
-        <v>646</v>
+        <v>662</v>
       </c>
       <c r="C256" t="s">
-        <v>647</v>
+        <v>663</v>
       </c>
       <c r="D256">
         <v>0</v>
@@ -8938,18 +9071,18 @@
         <v>0.55212772253787867</v>
       </c>
       <c r="G256">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="257" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8">
       <c r="A257" t="s">
-        <v>648</v>
+        <v>664</v>
       </c>
       <c r="B257" t="s">
-        <v>649</v>
+        <v>665</v>
       </c>
       <c r="C257" t="s">
-        <v>650</v>
+        <v>666</v>
       </c>
       <c r="D257">
         <v>0</v>
@@ -8961,18 +9094,18 @@
         <v>0.55186559491960985</v>
       </c>
       <c r="G257">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="258" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8">
       <c r="A258" t="s">
-        <v>651</v>
+        <v>667</v>
       </c>
       <c r="B258" t="s">
-        <v>652</v>
+        <v>668</v>
       </c>
       <c r="C258" t="s">
-        <v>653</v>
+        <v>669</v>
       </c>
       <c r="D258">
         <v>0</v>
@@ -8986,16 +9119,19 @@
       <c r="G258">
         <v>0</v>
       </c>
-    </row>
-    <row r="259" spans="1:7">
+      <c r="H258" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8">
       <c r="A259" t="s">
-        <v>654</v>
+        <v>671</v>
       </c>
       <c r="B259" t="s">
-        <v>655</v>
+        <v>672</v>
       </c>
       <c r="C259" t="s">
-        <v>656</v>
+        <v>673</v>
       </c>
       <c r="D259">
         <v>0</v>
@@ -9007,18 +9143,21 @@
         <v>0.41822372462464602</v>
       </c>
       <c r="G259">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="260" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H259" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8">
       <c r="A260" t="s">
-        <v>657</v>
+        <v>675</v>
       </c>
       <c r="B260" t="s">
-        <v>658</v>
+        <v>676</v>
       </c>
       <c r="C260" t="s">
-        <v>659</v>
+        <v>677</v>
       </c>
       <c r="D260">
         <v>0</v>
@@ -9032,16 +9171,19 @@
       <c r="G260">
         <v>0</v>
       </c>
-    </row>
-    <row r="261" spans="1:7">
+      <c r="H260" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8">
       <c r="A261" t="s">
-        <v>660</v>
+        <v>679</v>
       </c>
       <c r="B261" t="s">
-        <v>661</v>
+        <v>680</v>
       </c>
       <c r="C261" t="s">
-        <v>662</v>
+        <v>681</v>
       </c>
       <c r="D261">
         <v>0</v>
@@ -9056,15 +9198,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:7">
+    <row r="262" spans="1:8">
       <c r="A262" t="s">
-        <v>663</v>
+        <v>682</v>
       </c>
       <c r="B262" t="s">
-        <v>664</v>
+        <v>683</v>
       </c>
       <c r="C262" t="s">
-        <v>665</v>
+        <v>684</v>
       </c>
       <c r="D262">
         <v>0</v>
@@ -9079,15 +9221,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:7">
+    <row r="263" spans="1:8">
       <c r="A263" t="s">
-        <v>666</v>
+        <v>685</v>
       </c>
       <c r="B263" t="s">
-        <v>667</v>
+        <v>686</v>
       </c>
       <c r="C263" t="s">
-        <v>668</v>
+        <v>687</v>
       </c>
       <c r="D263">
         <v>0</v>
@@ -9102,15 +9244,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:7">
+    <row r="264" spans="1:8">
       <c r="A264" t="s">
-        <v>669</v>
+        <v>688</v>
       </c>
       <c r="B264" t="s">
-        <v>670</v>
+        <v>689</v>
       </c>
       <c r="C264" t="s">
-        <v>671</v>
+        <v>690</v>
       </c>
       <c r="D264">
         <v>0</v>
@@ -9125,15 +9267,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:7">
+    <row r="265" spans="1:8">
       <c r="A265" t="s">
-        <v>672</v>
+        <v>691</v>
       </c>
       <c r="B265" t="s">
-        <v>673</v>
+        <v>692</v>
       </c>
       <c r="C265" t="s">
-        <v>674</v>
+        <v>693</v>
       </c>
       <c r="D265">
         <v>0</v>
@@ -9148,15 +9290,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:7">
+    <row r="266" spans="1:8">
       <c r="A266" t="s">
-        <v>675</v>
+        <v>694</v>
       </c>
       <c r="B266" t="s">
-        <v>676</v>
+        <v>695</v>
       </c>
       <c r="C266" t="s">
-        <v>677</v>
+        <v>696</v>
       </c>
       <c r="D266">
         <v>0</v>
@@ -9171,15 +9313,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:7">
+    <row r="267" spans="1:8">
       <c r="A267" t="s">
-        <v>678</v>
+        <v>697</v>
       </c>
       <c r="B267" t="s">
-        <v>679</v>
+        <v>698</v>
       </c>
       <c r="C267" t="s">
-        <v>680</v>
+        <v>699</v>
       </c>
       <c r="D267">
         <v>0</v>
@@ -9194,15 +9336,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:7">
+    <row r="268" spans="1:8">
       <c r="A268" t="s">
-        <v>681</v>
+        <v>700</v>
       </c>
       <c r="B268" t="s">
-        <v>682</v>
+        <v>701</v>
       </c>
       <c r="C268" t="s">
-        <v>683</v>
+        <v>702</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -9217,15 +9359,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:7">
+    <row r="269" spans="1:8">
       <c r="A269" t="s">
-        <v>684</v>
+        <v>703</v>
       </c>
       <c r="B269" t="s">
-        <v>685</v>
+        <v>704</v>
       </c>
       <c r="C269" t="s">
-        <v>686</v>
+        <v>705</v>
       </c>
       <c r="D269">
         <v>0</v>
@@ -9240,15 +9382,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:7">
+    <row r="270" spans="1:8">
       <c r="A270" t="s">
-        <v>687</v>
+        <v>706</v>
       </c>
       <c r="B270" t="s">
-        <v>688</v>
+        <v>707</v>
       </c>
       <c r="C270" t="s">
-        <v>689</v>
+        <v>708</v>
       </c>
       <c r="D270">
         <v>0</v>
@@ -9263,15 +9405,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:7">
+    <row r="271" spans="1:8">
       <c r="A271" t="s">
-        <v>690</v>
+        <v>709</v>
       </c>
       <c r="B271" t="s">
-        <v>691</v>
+        <v>710</v>
       </c>
       <c r="C271" t="s">
-        <v>692</v>
+        <v>711</v>
       </c>
       <c r="D271">
         <v>0</v>
@@ -9286,15 +9428,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:7">
+    <row r="272" spans="1:8">
       <c r="A272" t="s">
-        <v>693</v>
+        <v>712</v>
       </c>
       <c r="B272" t="s">
-        <v>694</v>
+        <v>713</v>
       </c>
       <c r="C272" t="s">
-        <v>695</v>
+        <v>714</v>
       </c>
       <c r="D272">
         <v>0</v>
@@ -9311,13 +9453,13 @@
     </row>
     <row r="273" spans="1:7">
       <c r="A273" t="s">
-        <v>696</v>
+        <v>715</v>
       </c>
       <c r="B273" t="s">
-        <v>697</v>
+        <v>716</v>
       </c>
       <c r="C273" t="s">
-        <v>698</v>
+        <v>717</v>
       </c>
       <c r="D273">
         <v>0</v>
@@ -9334,13 +9476,13 @@
     </row>
     <row r="274" spans="1:7">
       <c r="A274" t="s">
-        <v>699</v>
+        <v>718</v>
       </c>
       <c r="B274" t="s">
-        <v>700</v>
+        <v>719</v>
       </c>
       <c r="C274" t="s">
-        <v>701</v>
+        <v>720</v>
       </c>
       <c r="D274">
         <v>0</v>
@@ -9357,13 +9499,13 @@
     </row>
     <row r="275" spans="1:7">
       <c r="A275" t="s">
-        <v>702</v>
+        <v>721</v>
       </c>
       <c r="B275" t="s">
-        <v>703</v>
+        <v>722</v>
       </c>
       <c r="C275" t="s">
-        <v>704</v>
+        <v>723</v>
       </c>
       <c r="D275">
         <v>0</v>
@@ -9380,13 +9522,13 @@
     </row>
     <row r="276" spans="1:7">
       <c r="A276" t="s">
-        <v>705</v>
+        <v>724</v>
       </c>
       <c r="B276" t="s">
-        <v>706</v>
+        <v>725</v>
       </c>
       <c r="C276" t="s">
-        <v>707</v>
+        <v>726</v>
       </c>
       <c r="D276">
         <v>0</v>
@@ -9403,13 +9545,13 @@
     </row>
     <row r="277" spans="1:7">
       <c r="A277" t="s">
-        <v>708</v>
+        <v>727</v>
       </c>
       <c r="B277" t="s">
-        <v>709</v>
+        <v>728</v>
       </c>
       <c r="C277" t="s">
-        <v>710</v>
+        <v>729</v>
       </c>
       <c r="D277">
         <v>0</v>
@@ -9426,13 +9568,13 @@
     </row>
     <row r="278" spans="1:7">
       <c r="A278" t="s">
-        <v>711</v>
+        <v>730</v>
       </c>
       <c r="B278" t="s">
-        <v>712</v>
+        <v>731</v>
       </c>
       <c r="C278" t="s">
-        <v>712</v>
+        <v>731</v>
       </c>
       <c r="D278">
         <v>1</v>
@@ -9449,13 +9591,13 @@
     </row>
     <row r="279" spans="1:7">
       <c r="A279" t="s">
-        <v>713</v>
+        <v>732</v>
       </c>
       <c r="B279" t="s">
-        <v>714</v>
+        <v>733</v>
       </c>
       <c r="C279" t="s">
-        <v>715</v>
+        <v>734</v>
       </c>
       <c r="D279">
         <v>0</v>
@@ -9472,13 +9614,13 @@
     </row>
     <row r="280" spans="1:7">
       <c r="A280" t="s">
-        <v>716</v>
+        <v>735</v>
       </c>
       <c r="B280" t="s">
-        <v>717</v>
+        <v>736</v>
       </c>
       <c r="C280" t="s">
-        <v>717</v>
+        <v>736</v>
       </c>
       <c r="D280">
         <v>1</v>
@@ -9495,13 +9637,13 @@
     </row>
     <row r="281" spans="1:7">
       <c r="A281" t="s">
-        <v>718</v>
+        <v>737</v>
       </c>
       <c r="B281" t="s">
-        <v>719</v>
+        <v>738</v>
       </c>
       <c r="C281" t="s">
-        <v>720</v>
+        <v>739</v>
       </c>
       <c r="D281">
         <v>0</v>
@@ -9518,13 +9660,13 @@
     </row>
     <row r="282" spans="1:7">
       <c r="A282" t="s">
-        <v>721</v>
+        <v>740</v>
       </c>
       <c r="B282" t="s">
-        <v>722</v>
+        <v>741</v>
       </c>
       <c r="C282" t="s">
-        <v>722</v>
+        <v>741</v>
       </c>
       <c r="D282">
         <v>1</v>
@@ -9541,13 +9683,13 @@
     </row>
     <row r="283" spans="1:7">
       <c r="A283" t="s">
-        <v>723</v>
+        <v>742</v>
       </c>
       <c r="B283" t="s">
-        <v>724</v>
+        <v>743</v>
       </c>
       <c r="C283" t="s">
-        <v>725</v>
+        <v>744</v>
       </c>
       <c r="D283">
         <v>0</v>
@@ -9564,13 +9706,13 @@
     </row>
     <row r="284" spans="1:7">
       <c r="A284" t="s">
-        <v>726</v>
+        <v>745</v>
       </c>
       <c r="B284" t="s">
-        <v>727</v>
+        <v>746</v>
       </c>
       <c r="C284" t="s">
-        <v>728</v>
+        <v>747</v>
       </c>
       <c r="D284">
         <v>1</v>
@@ -9587,13 +9729,13 @@
     </row>
     <row r="285" spans="1:7">
       <c r="A285" t="s">
-        <v>729</v>
+        <v>748</v>
       </c>
       <c r="B285" t="s">
-        <v>730</v>
+        <v>749</v>
       </c>
       <c r="C285" t="s">
-        <v>730</v>
+        <v>749</v>
       </c>
       <c r="D285">
         <v>1</v>
@@ -9610,13 +9752,13 @@
     </row>
     <row r="286" spans="1:7">
       <c r="A286" t="s">
-        <v>731</v>
+        <v>750</v>
       </c>
       <c r="B286" t="s">
-        <v>732</v>
+        <v>751</v>
       </c>
       <c r="C286" t="s">
-        <v>733</v>
+        <v>752</v>
       </c>
       <c r="D286">
         <v>0</v>
@@ -9633,13 +9775,13 @@
     </row>
     <row r="287" spans="1:7">
       <c r="A287" t="s">
-        <v>734</v>
+        <v>753</v>
       </c>
       <c r="B287" t="s">
-        <v>735</v>
+        <v>754</v>
       </c>
       <c r="C287" t="s">
-        <v>736</v>
+        <v>755</v>
       </c>
       <c r="D287">
         <v>0</v>
@@ -9656,13 +9798,13 @@
     </row>
     <row r="288" spans="1:7">
       <c r="A288" t="s">
-        <v>737</v>
+        <v>756</v>
       </c>
       <c r="B288" t="s">
-        <v>738</v>
+        <v>757</v>
       </c>
       <c r="C288" t="s">
-        <v>739</v>
+        <v>758</v>
       </c>
       <c r="D288">
         <v>0</v>
@@ -9679,13 +9821,13 @@
     </row>
     <row r="289" spans="1:7">
       <c r="A289" t="s">
-        <v>740</v>
+        <v>759</v>
       </c>
       <c r="B289" t="s">
-        <v>741</v>
+        <v>760</v>
       </c>
       <c r="C289" t="s">
-        <v>742</v>
+        <v>761</v>
       </c>
       <c r="D289">
         <v>0</v>
@@ -9702,13 +9844,13 @@
     </row>
     <row r="290" spans="1:7">
       <c r="A290" t="s">
-        <v>743</v>
+        <v>762</v>
       </c>
       <c r="B290" t="s">
-        <v>744</v>
+        <v>763</v>
       </c>
       <c r="C290" t="s">
-        <v>745</v>
+        <v>764</v>
       </c>
       <c r="D290">
         <v>0</v>
@@ -9725,13 +9867,13 @@
     </row>
     <row r="291" spans="1:7">
       <c r="A291" t="s">
-        <v>746</v>
+        <v>765</v>
       </c>
       <c r="B291" t="s">
-        <v>747</v>
+        <v>766</v>
       </c>
       <c r="C291" t="s">
-        <v>748</v>
+        <v>767</v>
       </c>
       <c r="D291">
         <v>0</v>
@@ -9748,13 +9890,13 @@
     </row>
     <row r="292" spans="1:7">
       <c r="A292" t="s">
-        <v>749</v>
+        <v>768</v>
       </c>
       <c r="B292" t="s">
-        <v>750</v>
+        <v>769</v>
       </c>
       <c r="C292" t="s">
-        <v>751</v>
+        <v>770</v>
       </c>
       <c r="D292">
         <v>0</v>
@@ -9771,13 +9913,13 @@
     </row>
     <row r="293" spans="1:7">
       <c r="A293" t="s">
-        <v>752</v>
+        <v>771</v>
       </c>
       <c r="B293" t="s">
-        <v>753</v>
+        <v>772</v>
       </c>
       <c r="C293" t="s">
-        <v>753</v>
+        <v>772</v>
       </c>
       <c r="D293">
         <v>1</v>
@@ -9794,13 +9936,13 @@
     </row>
     <row r="294" spans="1:7">
       <c r="A294" t="s">
-        <v>754</v>
+        <v>773</v>
       </c>
       <c r="B294" t="s">
-        <v>755</v>
+        <v>774</v>
       </c>
       <c r="C294" t="s">
-        <v>756</v>
+        <v>775</v>
       </c>
       <c r="D294">
         <v>0</v>
@@ -9817,13 +9959,13 @@
     </row>
     <row r="295" spans="1:7">
       <c r="A295" t="s">
-        <v>757</v>
+        <v>776</v>
       </c>
       <c r="B295" t="s">
-        <v>758</v>
+        <v>777</v>
       </c>
       <c r="C295" t="s">
-        <v>759</v>
+        <v>778</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -9840,13 +9982,13 @@
     </row>
     <row r="296" spans="1:7">
       <c r="A296" t="s">
-        <v>760</v>
+        <v>779</v>
       </c>
       <c r="B296" t="s">
-        <v>761</v>
+        <v>780</v>
       </c>
       <c r="C296" t="s">
-        <v>762</v>
+        <v>781</v>
       </c>
       <c r="D296">
         <v>0</v>
@@ -9863,13 +10005,13 @@
     </row>
     <row r="297" spans="1:7">
       <c r="A297" t="s">
-        <v>763</v>
+        <v>782</v>
       </c>
       <c r="B297" t="s">
-        <v>764</v>
+        <v>783</v>
       </c>
       <c r="C297" t="s">
-        <v>765</v>
+        <v>784</v>
       </c>
       <c r="D297">
         <v>0</v>
@@ -9886,13 +10028,13 @@
     </row>
     <row r="298" spans="1:7">
       <c r="A298" t="s">
-        <v>766</v>
+        <v>785</v>
       </c>
       <c r="B298" t="s">
-        <v>767</v>
+        <v>786</v>
       </c>
       <c r="C298" t="s">
-        <v>768</v>
+        <v>787</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -9909,13 +10051,13 @@
     </row>
     <row r="299" spans="1:7">
       <c r="A299" t="s">
-        <v>769</v>
+        <v>788</v>
       </c>
       <c r="B299" t="s">
-        <v>770</v>
+        <v>789</v>
       </c>
       <c r="C299" t="s">
-        <v>770</v>
+        <v>789</v>
       </c>
       <c r="D299">
         <v>1</v>
@@ -9932,13 +10074,13 @@
     </row>
     <row r="300" spans="1:7">
       <c r="A300" t="s">
-        <v>771</v>
+        <v>790</v>
       </c>
       <c r="B300" t="s">
-        <v>772</v>
+        <v>791</v>
       </c>
       <c r="C300" t="s">
-        <v>772</v>
+        <v>791</v>
       </c>
       <c r="D300">
         <v>1</v>
@@ -9955,13 +10097,13 @@
     </row>
     <row r="301" spans="1:7">
       <c r="A301" t="s">
-        <v>773</v>
+        <v>792</v>
       </c>
       <c r="B301" t="s">
-        <v>774</v>
+        <v>793</v>
       </c>
       <c r="C301" t="s">
-        <v>775</v>
+        <v>794</v>
       </c>
       <c r="D301">
         <v>0</v>
@@ -9978,13 +10120,13 @@
     </row>
     <row r="302" spans="1:7">
       <c r="A302" t="s">
-        <v>776</v>
+        <v>795</v>
       </c>
       <c r="B302" t="s">
-        <v>777</v>
+        <v>796</v>
       </c>
       <c r="C302" t="s">
-        <v>778</v>
+        <v>797</v>
       </c>
       <c r="D302">
         <v>0</v>
@@ -10001,13 +10143,13 @@
     </row>
     <row r="303" spans="1:7">
       <c r="A303" t="s">
-        <v>779</v>
+        <v>798</v>
       </c>
       <c r="B303" t="s">
-        <v>780</v>
+        <v>799</v>
       </c>
       <c r="C303" t="s">
-        <v>781</v>
+        <v>800</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -10024,13 +10166,13 @@
     </row>
     <row r="304" spans="1:7">
       <c r="A304" t="s">
-        <v>782</v>
+        <v>801</v>
       </c>
       <c r="B304" t="s">
-        <v>783</v>
+        <v>802</v>
       </c>
       <c r="C304" t="s">
-        <v>784</v>
+        <v>803</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -10047,13 +10189,13 @@
     </row>
     <row r="305" spans="1:7">
       <c r="A305" t="s">
-        <v>785</v>
+        <v>804</v>
       </c>
       <c r="B305" t="s">
-        <v>786</v>
+        <v>805</v>
       </c>
       <c r="C305" t="s">
-        <v>787</v>
+        <v>806</v>
       </c>
       <c r="D305">
         <v>0</v>
@@ -10070,13 +10212,13 @@
     </row>
     <row r="306" spans="1:7">
       <c r="A306" t="s">
-        <v>788</v>
+        <v>807</v>
       </c>
       <c r="B306" t="s">
-        <v>789</v>
+        <v>808</v>
       </c>
       <c r="C306" t="s">
-        <v>790</v>
+        <v>809</v>
       </c>
       <c r="D306">
         <v>0</v>
@@ -10093,13 +10235,13 @@
     </row>
     <row r="307" spans="1:7">
       <c r="A307" t="s">
-        <v>791</v>
+        <v>810</v>
       </c>
       <c r="B307" t="s">
-        <v>792</v>
+        <v>811</v>
       </c>
       <c r="C307" t="s">
-        <v>793</v>
+        <v>812</v>
       </c>
       <c r="D307">
         <v>0</v>
@@ -10116,13 +10258,13 @@
     </row>
     <row r="308" spans="1:7">
       <c r="A308" t="s">
-        <v>794</v>
+        <v>813</v>
       </c>
       <c r="B308" t="s">
-        <v>795</v>
+        <v>814</v>
       </c>
       <c r="C308" t="s">
-        <v>796</v>
+        <v>815</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -10139,13 +10281,13 @@
     </row>
     <row r="309" spans="1:7">
       <c r="A309" t="s">
-        <v>797</v>
+        <v>816</v>
       </c>
       <c r="B309" t="s">
-        <v>798</v>
+        <v>817</v>
       </c>
       <c r="C309" t="s">
-        <v>799</v>
+        <v>818</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -10162,13 +10304,13 @@
     </row>
     <row r="310" spans="1:7">
       <c r="A310" t="s">
-        <v>800</v>
+        <v>819</v>
       </c>
       <c r="B310" t="s">
-        <v>801</v>
+        <v>820</v>
       </c>
       <c r="C310" t="s">
-        <v>801</v>
+        <v>820</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -10185,13 +10327,13 @@
     </row>
     <row r="311" spans="1:7">
       <c r="A311" t="s">
-        <v>802</v>
+        <v>821</v>
       </c>
       <c r="B311" t="s">
-        <v>803</v>
+        <v>822</v>
       </c>
       <c r="C311" t="s">
-        <v>803</v>
+        <v>822</v>
       </c>
       <c r="D311">
         <v>1</v>
@@ -10208,13 +10350,13 @@
     </row>
     <row r="312" spans="1:7">
       <c r="A312" t="s">
-        <v>804</v>
+        <v>823</v>
       </c>
       <c r="B312" t="s">
-        <v>805</v>
+        <v>824</v>
       </c>
       <c r="C312" t="s">
-        <v>806</v>
+        <v>825</v>
       </c>
       <c r="D312">
         <v>0</v>
@@ -10231,13 +10373,13 @@
     </row>
     <row r="313" spans="1:7">
       <c r="A313" t="s">
-        <v>807</v>
+        <v>826</v>
       </c>
       <c r="B313" t="s">
-        <v>808</v>
+        <v>827</v>
       </c>
       <c r="C313" t="s">
-        <v>809</v>
+        <v>828</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -10254,13 +10396,13 @@
     </row>
     <row r="314" spans="1:7">
       <c r="A314" t="s">
-        <v>810</v>
+        <v>829</v>
       </c>
       <c r="B314" t="s">
-        <v>811</v>
+        <v>830</v>
       </c>
       <c r="C314" t="s">
-        <v>812</v>
+        <v>831</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -10277,13 +10419,13 @@
     </row>
     <row r="315" spans="1:7">
       <c r="A315" t="s">
-        <v>813</v>
+        <v>832</v>
       </c>
       <c r="B315" t="s">
-        <v>814</v>
+        <v>833</v>
       </c>
       <c r="C315" t="s">
-        <v>815</v>
+        <v>834</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -10300,13 +10442,13 @@
     </row>
     <row r="316" spans="1:7">
       <c r="A316" t="s">
-        <v>816</v>
+        <v>835</v>
       </c>
       <c r="B316" t="s">
-        <v>817</v>
+        <v>836</v>
       </c>
       <c r="C316" t="s">
-        <v>818</v>
+        <v>837</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -10323,13 +10465,13 @@
     </row>
     <row r="317" spans="1:7">
       <c r="A317" t="s">
-        <v>819</v>
+        <v>838</v>
       </c>
       <c r="B317" t="s">
-        <v>820</v>
+        <v>839</v>
       </c>
       <c r="C317" t="s">
-        <v>821</v>
+        <v>840</v>
       </c>
       <c r="D317">
         <v>0</v>
@@ -10346,13 +10488,13 @@
     </row>
     <row r="318" spans="1:7">
       <c r="A318" t="s">
-        <v>822</v>
+        <v>841</v>
       </c>
       <c r="B318" t="s">
-        <v>823</v>
+        <v>842</v>
       </c>
       <c r="C318" t="s">
-        <v>824</v>
+        <v>843</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -10369,13 +10511,13 @@
     </row>
     <row r="319" spans="1:7">
       <c r="A319" t="s">
-        <v>825</v>
+        <v>844</v>
       </c>
       <c r="B319" t="s">
-        <v>826</v>
+        <v>845</v>
       </c>
       <c r="C319" t="s">
-        <v>827</v>
+        <v>846</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -10392,13 +10534,13 @@
     </row>
     <row r="320" spans="1:7">
       <c r="A320" t="s">
-        <v>828</v>
+        <v>847</v>
       </c>
       <c r="B320" t="s">
-        <v>829</v>
+        <v>848</v>
       </c>
       <c r="C320" t="s">
-        <v>830</v>
+        <v>849</v>
       </c>
       <c r="D320">
         <v>0</v>
@@ -10415,13 +10557,13 @@
     </row>
     <row r="321" spans="1:7">
       <c r="A321" t="s">
-        <v>831</v>
+        <v>850</v>
       </c>
       <c r="B321" t="s">
-        <v>832</v>
+        <v>851</v>
       </c>
       <c r="C321" t="s">
-        <v>832</v>
+        <v>851</v>
       </c>
       <c r="D321">
         <v>1</v>
@@ -10438,13 +10580,13 @@
     </row>
     <row r="322" spans="1:7">
       <c r="A322" t="s">
-        <v>833</v>
+        <v>852</v>
       </c>
       <c r="B322" t="s">
-        <v>834</v>
+        <v>853</v>
       </c>
       <c r="C322" t="s">
-        <v>834</v>
+        <v>853</v>
       </c>
       <c r="D322">
         <v>1</v>
@@ -10461,13 +10603,13 @@
     </row>
     <row r="323" spans="1:7">
       <c r="A323" t="s">
-        <v>835</v>
+        <v>854</v>
       </c>
       <c r="B323" t="s">
-        <v>836</v>
+        <v>855</v>
       </c>
       <c r="C323" t="s">
-        <v>836</v>
+        <v>855</v>
       </c>
       <c r="D323">
         <v>1</v>
@@ -10484,13 +10626,13 @@
     </row>
     <row r="324" spans="1:7">
       <c r="A324" t="s">
-        <v>837</v>
+        <v>856</v>
       </c>
       <c r="B324" t="s">
-        <v>838</v>
+        <v>857</v>
       </c>
       <c r="C324" t="s">
-        <v>839</v>
+        <v>858</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -10507,13 +10649,13 @@
     </row>
     <row r="325" spans="1:7">
       <c r="A325" t="s">
-        <v>840</v>
+        <v>859</v>
       </c>
       <c r="B325" t="s">
-        <v>841</v>
+        <v>860</v>
       </c>
       <c r="C325" t="s">
-        <v>842</v>
+        <v>861</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -10530,13 +10672,13 @@
     </row>
     <row r="326" spans="1:7">
       <c r="A326" t="s">
-        <v>843</v>
+        <v>862</v>
       </c>
       <c r="B326" t="s">
-        <v>844</v>
+        <v>863</v>
       </c>
       <c r="C326" t="s">
-        <v>844</v>
+        <v>863</v>
       </c>
       <c r="D326">
         <v>1</v>
@@ -10553,13 +10695,13 @@
     </row>
     <row r="327" spans="1:7">
       <c r="A327" t="s">
-        <v>845</v>
+        <v>864</v>
       </c>
       <c r="B327" t="s">
-        <v>846</v>
+        <v>865</v>
       </c>
       <c r="C327" t="s">
-        <v>846</v>
+        <v>865</v>
       </c>
       <c r="D327">
         <v>1</v>

</xml_diff>

<commit_message>
Aggiunte nuove analisi e tempi di valutazione
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/AnalisiCodeGen.xlsx
+++ b/HE/W_in_progress/AnalisiCodeGen.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28209"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8AA68D5-BF92-4DC9-8954-CA6483AFA676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A141B2D-AF37-4311-AC6B-159E6CFFA02F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="882">
   <si>
     <t>IN</t>
   </si>
@@ -2097,6 +2097,27 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity dual_port_ram is Generic(K : integer := 8; L : integer := 32); Port ( Clock : in STD_LOGIC; Write_Enable : in STD_LOGIC; Read_Enable : in STD_LOGIC; Write_Address : in STD_LOGIC_VECTOR (log2K-1 downto 0); Read_Address : in STD_LOGIC_VECTOR (log2K-1 downto 0); Data_In : in STD_LOGIC_VECTOR (L-1 downto 0); Data_Out : out STD_LOGIC_VECTOR (L-1 downto 0)); end dual_port_ram; architecture Behavioral of dual_port_ram is type ram_type is array (0 to K-1) of std_logic_vector(L-1 downto 0); signal ram : ram_type; begin process (Clock) begin if rising_edge(Clock) then if Write_Enable = '1' then ram(Write_Address) &lt;= Data_In; end if ; if Read_Enable = '1' then Data_Out &lt;= ram(Read_Address); end if ; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Contiene un errore sintattico ma tolto quello è corretto </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(log2K-1)</t>
+    </r>
+  </si>
+  <si>
     <t>Generate a dual-port memory of K x L with the signals clock, write, address_w (log2K-bit), address_r (log2K-bit), and data_write (L-bit) as input and the signal data_read (L-bit) as output.</t>
   </si>
   <si>
@@ -2106,6 +2127,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity dual_port_memory is Generic(K : integer := 8; L : integer := 32); Port ( Clock : in STD_LOGIC; Write : in STD_LOGIC; Address_W : in STD_LOGIC_VECTOR (log2K-1 downto 0); Address_R : in STD_LOGIC_VECTOR (log2K-1 downto 0); Data_Write : in STD_LOGIC_VECTOR (L-1 downto 0); Data_Read : out STD_LOGIC_VECTOR (L-1 downto 0)); end dual_port_memory; architecture Behavioral of dual_port_memory is type mem_array is array (0 to K-1) of std_logic_vector(L-1 downto 0); signal memory : mem_array := (others =&gt; (others =&gt; '0')); begin process (Clock, Write, Address_W, Data_Write) begin if rising_edge(Clock) then if Write = '1' then memory(to_integer(unsigned(Address_W))) &lt;= Data_Write; end if ; end if ; end process ; Data_Read &lt;= memory(to_integer(unsigned(Address_R))); end Behavioral;</t>
   </si>
   <si>
+    <t>La do buona anche se ci sarebbero delle correzioni da fare</t>
+  </si>
+  <si>
     <t>Create a 4-bit binary counter that increments on each clock pulse and resets asynchronously</t>
   </si>
   <si>
@@ -2124,6 +2148,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity fir_filter is Generic ( N : natural := 8; M : natural := 5 ); Port ( Clock : in STD_LOGIC; Reset : in STD_LOGIC; Data_In : in signed(N-1 downto 0); Coefficients : in signed(M*N-1 downto 0); Filtered_Output : out signed(N-1 downto 0) ); end fir_filter; architecture Behavioral of fir_filter is signal accumulator : signed(M*N downto 0) := (others =&gt; '0'); begin process (Clock, Reset) begin if Reset = '1' then accumulator &lt;= (others =&gt; '0'); elsif rising_edge(Clock) then for i in 0 to M-1 loop accumulator(i) &lt;= accumulator(i) xor Data_In; end loop ; end if ; end process ; Filtered_Output &lt;= accumulator(N-1 downto 0); end Behavioral;</t>
   </si>
   <si>
+    <t xml:space="preserve">Semanticamente simile </t>
+  </si>
+  <si>
     <t>Implement a basic clock gating circuit</t>
   </si>
   <si>
@@ -2133,6 +2160,9 @@
     <t>process(clk, rst) begin if rst = '1' then q &lt;= '0'; elsif rising_edge(clk) then if q = '0' then q &lt;= '1'; else q &lt;= '0'; end if; end if; end process;</t>
   </si>
   <si>
+    <t>Non fa il clock gating, ma un flip-flop</t>
+  </si>
+  <si>
     <t>Write a floating-point multiplier of N-bit with the signals A (N-bit) and B (N-bit) as input and the signal product (N-bit) as output.</t>
   </si>
   <si>
@@ -2142,6 +2172,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity Floating_Point_Multiplier is Generic (N : natural := 32); Port (A : in STD_LOGIC_VECTOR (N-1 downto 0); B : in STD_LOGIC_VECTOR (N-1 downto 0); Product : out STD_LOGIC_VECTOR (N-1 downto 0)); end Floating_Point_Multiplier; architecture Behavioral of Floating_Point_Multiplier is signal A_float, B_float, Product_float : float32; begin A_float &lt;= to_float(A, 8, 23); B_float &lt;= to_float(B, 8, 23); Product_float &lt;= A_float * B_float; Product &lt;= to_slv(Product_float); end Behavioral;</t>
   </si>
   <si>
+    <t xml:space="preserve">Necessita di funzioni specifiche però grossomodo ci sta </t>
+  </si>
+  <si>
     <t>Define a BCD to binary converter of (N/3)+1-digit with the signal BCD_value ((N/3)+1-digit) as input and the signal binary_value (N-bit) as output.</t>
   </si>
   <si>
@@ -2151,6 +2184,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity BCD_to_Binary is Generic (N : integer := 8); Port (BCD_Value : in STD_LOGIC_VECTOR ((N/3)+1-1 downto 0); Binary_Value : out STD_LOGIC_VECTOR (N-1 downto 0)); end BCD_to_Binary; architecture Behavioral of BCD_to_Binary is begin process (BCD_Value) variable temp : STD_LOGIC_VECTOR ((N/3)+1-1 downto 0); begin for i in 0 to N/3 loop temp(i) := BCD_Value((i+1)*3-1 downto i*3); end loop ; Binary_Value &lt;= temp; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t xml:space="preserve">Non esegue la conversione </t>
+  </si>
+  <si>
     <t>Create a basic frequency meter</t>
   </si>
   <si>
@@ -2169,6 +2205,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity Digital_Differentiator is Generic ( N : natural := 8 ); Port ( Clk : in STD_LOGIC; Input_Data : in STD_LOGIC_VECTOR (N-1 downto 0); Differentiated_Data : out STD_LOGIC_VECTOR (N-1 downto 0)); end Digital_Differentiator; architecture Behavioral of Digital_Differentiator is signal Differentiated_Data_Reg : STD_LOGIC_VECTOR (N-1 downto 0); begin process (Clk) begin if rising_edge(Clk) then Differentiated_Data_Reg &lt;= Input_Data; end if ; end process ; Differentiated_Data &lt;= Differentiated_Data_Reg; end Behavioral;</t>
   </si>
   <si>
+    <t>Non effettua la differenziazione</t>
+  </si>
+  <si>
     <t>Define a digital integrator of N-bit with the signals clock, reset, and data_in (N-bit) as input and the signal integrated_output (N-bit) as output.</t>
   </si>
   <si>
@@ -2178,6 +2217,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity DigitalIntegrator is Generic ( N : natural := 8 ); Port ( Clock : in STD_LOGIC; Reset : in STD_LOGIC; Data_In : in STD_LOGIC_VECTOR (N-1 downto 0); Integrated_Output : out STD_LOGIC_VECTOR (N-1 downto 0)); end DigitalIntegrator; architecture Behavioral of DigitalIntegrator is signal Accumulator : STD_LOGIC_VECTOR (N-1 downto 0) := (others =&gt; '0'); begin process (Clock, Reset) begin if Reset = '1' then Accumulator &lt;= (others =&gt; '0'); elsif rising_edge(Clock) then Accumulator &lt;= Accumulator + Data_In; end if ; end process ; Integrated_Output &lt;= Accumulator; end Behavioral;</t>
   </si>
   <si>
+    <t>E' un differenziatore</t>
+  </si>
+  <si>
     <t>Define a CRC generator of N-bit with the signals data_in (N-bit) and polynomial (M-bit) as input and the signal CRC_value (M-bit) as output.</t>
   </si>
   <si>
@@ -2187,6 +2229,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity crc_generator is Generic (N : natural := 8; M : natural := 16); Port ( Data_In : in STD_LOGIC_VECTOR (N-1 downto 0); Polynomial : in STD_LOGIC_VECTOR (M-1 downto 0); CRC_Value : out STD_LOGIC_VECTOR (M-1 downto 0)); end crc_generator; architecture Behavioral of crc_generator is begin process (Data_In, Polynomial) variable temp_crc : STD_LOGIC_VECTOR (M-1 downto 0); begin temp_crc := (others =&gt; '0'); for i in 0 to N-1 loop if Data_In(i) = '1' then temp_crc := temp_crc xor Polynomial; end if ; end loop ; CRC_Value &lt;= temp_crc; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Un CRC non preciso, ma un CRC</t>
+  </si>
+  <si>
     <t>Generate a priority encoder of 2^M-to-M with the signal requests (2^M-bit) as input and the signals encoded (M-bit) and valid as output.</t>
   </si>
   <si>
@@ -2196,6 +2241,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity PriorityEncoder is Generic(M: integer := 2); Port ( Requests : in STD_LOGIC_VECTOR (2**M-1 downto 0); Encoded : out STD_LOGIC_VECTOR (M-1 downto 0); Valid : out STD_LOGIC); end PriorityEncoder; architecture Behavioral of PriorityEncoder is begin process (Requests) variable temp: std_logic_vector(2**M-1 downto 0); begin Valid &lt;= '0'; for i in Requests'range loop if Requests(2**i - 1) = '1' then Valid &lt;= '1'; end if ; end loop ; Encoded &lt;= temp; Valid &lt;= '1'; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non implementa correttemente l'encoder</t>
+  </si>
+  <si>
     <t>Define an unsigned divider of N-bit with the signals dividend (N-bit) and divisor (N-bit) as input and the signals quotient (N-bit) and remainder (N-bit) as output.</t>
   </si>
   <si>
@@ -2205,6 +2253,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity UnsignedDivider is Generic (N : natural := 8); Port ( Dividend : in STD_LOGIC_VECTOR (N-1 downto 0); Divisor : in STD_LOGIC_VECTOR (N-1 downto 0); Quotient : out STD_LOGIC_VECTOR (N-1 downto 0); Remainder : out STD_LOGIC_VECTOR (N-1 downto 0)); end UnsignedDivider; architecture Behavioral of UnsignedDivider is begin process (Dividend, Divisor) variable temp_quotient : STD_LOGIC_VECTOR (N-1 downto 0); variable temp_remainder : STD_LOGIC_VECTOR (N-1 downto 0); begin temp_quotient := (others =&gt; '0'); temp_remainder := Dividend; for i in 0 to N-1 loop if temp_remainder &gt;= Divisor then temp_quotient(i) := '1'; temp_remainder := temp_remainder - Divisor; end if ; end loop ; Quotient &lt;= temp_quotient; Remainder &lt;= temp_remainder; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Vanno aggiustate un po di cose, ma la semantica va bene</t>
+  </si>
+  <si>
     <t>Implement a basic I2C master controller</t>
   </si>
   <si>
@@ -2214,6 +2265,9 @@
     <t>process(clk) begin if rising_edge(clk) then case state is when IDLE =&gt; if start = '1' then state &lt;= START_BIT; bit_count &lt;= 0; when START_BIT =&gt; sclk &lt;= '0'; if bit_timer = BIT_PERIOD - 1 then sda_out &lt;= '0'; bit_timer &lt;= 0; else bit_timer &lt;= bit_timer + 1; end if; when STOP_BIT =&gt; sclk &lt;= '1'; if bit_timer = BIT_PERIOD - 1 then sda_out &lt;= '1'; bit_timer &lt;= 0; else bit_timer &lt;= bit_timer + 1; end if; when IDLE =&gt; sclk &lt;= '0'; if bit_timer = BIT_PERIOD - 1 then sda_out &lt;= '0'; bit_timer &lt;= 0; else bit_timer &lt;= bit_timer + 1; end if; end case; end if; end process;</t>
   </si>
   <si>
+    <t>Implementa un I2C master controller</t>
+  </si>
+  <si>
     <t>Create a basic DDS (Direct Digital Synthesis) waveform generator</t>
   </si>
   <si>
@@ -2223,6 +2277,9 @@
     <t>process(clk) begin if rising_edge(clk) then if counter = DIV - 1 then phase_acc &lt;= phase_acc + phase_inc; sine_out &lt;= sine_lut(to_integer(phase_acc(31 downto 24))); cosine_out &lt;= cosine_lut(to_integer(phase_acc(31 downto 24))); end if; counter &lt;= 0; end if; end process;</t>
   </si>
   <si>
+    <t>Implementana un DDS (Direct Digital Synthesis) waveform generator</t>
+  </si>
+  <si>
     <t>Write a comparator circuit of K-bit with the signals value1 (K-bit) and value2 (K-bit) as input and the signals greater, equal, and smaller as output.</t>
   </si>
   <si>
@@ -2232,6 +2289,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity Comparator is Port ( Value1 : in STD_LOGIC_VECTOR (K-1 downto 0); Value2 : in STD_LOGIC_VECTOR (K-1 downto 0); Greater : out STD_LOGIC; Equal : out STD_LOGIC; Smaller : out STD_LOGIC); end Comparator; architecture Behavioral of Comparator is begin process (Value1, Value2) variable temp : STD_LOGIC_VECTOR (K-1 downto 0); begin temp := (Value1 &amp; Value2); Greater &lt;= temp(K-1) when Equal = '1' else '0'; Equal &lt;= temp(K-1) when Equal = '1' else '0'; Smaller &lt;= temp(K-1) when Equal = '1' else '0'; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non implementa un comparatore</t>
+  </si>
+  <si>
     <t>if rising edge of clk_i; when the case is other_st; set cathodes_dot signal to the concatenation of cathodes and the complement of dot signal</t>
   </si>
   <si>
@@ -2241,6 +2301,9 @@
     <t>if rising_edge(clk_i) then; when other_st =&gt;; cathodes_dot &lt;= (not dot)&amp;cathodes;</t>
   </si>
   <si>
+    <t>Sbagliata l'implementazione</t>
+  </si>
+  <si>
     <t>declare a signal t_tick_o of type std_logic; S signal is set to the result of an XOR operation between CIN and the XOR operation between OP_A and OP_B.</t>
   </si>
   <si>
@@ -2284,6 +2347,9 @@
   </si>
   <si>
     <t>constant CLK_DIV : integer := 100; signal prova : std_logic_vector(3 downto 0);</t>
+  </si>
+  <si>
+    <t>Non effettua la concatenazione</t>
   </si>
   <si>
     <t>i_cs_re_tk is a signal of type std_logic used for something related to rising edge and timekeeping; define an output std_logic_vector of 8 bit called anodes</t>
@@ -3026,8 +3092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="G261" sqref="G261"/>
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+      <selection activeCell="H283" sqref="H283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9195,18 +9261,21 @@
         <v>0.6489489332562548</v>
       </c>
       <c r="G261">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H261" s="3" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="262" spans="1:8">
       <c r="A262" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B262" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="C262" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="D262">
         <v>0</v>
@@ -9218,18 +9287,21 @@
         <v>0.78764365382535173</v>
       </c>
       <c r="G262">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H262" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="263" spans="1:8">
       <c r="A263" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="B263" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="C263" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="D263">
         <v>0</v>
@@ -9241,18 +9313,18 @@
         <v>0.93440094834565979</v>
       </c>
       <c r="G263">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="264" spans="1:8">
       <c r="A264" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="B264" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="C264" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="D264">
         <v>0</v>
@@ -9264,18 +9336,21 @@
         <v>0.54570147431668192</v>
       </c>
       <c r="G264">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H264" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="265" spans="1:8">
       <c r="A265" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="B265" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="C265" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="D265">
         <v>0</v>
@@ -9289,16 +9364,19 @@
       <c r="G265">
         <v>0</v>
       </c>
+      <c r="H265" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="266" spans="1:8">
       <c r="A266" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
       <c r="B266" t="s">
-        <v>695</v>
+        <v>699</v>
       </c>
       <c r="C266" t="s">
-        <v>696</v>
+        <v>700</v>
       </c>
       <c r="D266">
         <v>0</v>
@@ -9310,18 +9388,21 @@
         <v>0.6536978520598028</v>
       </c>
       <c r="G266">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H266" t="s">
+        <v>701</v>
       </c>
     </row>
     <row r="267" spans="1:8">
       <c r="A267" t="s">
-        <v>697</v>
+        <v>702</v>
       </c>
       <c r="B267" t="s">
-        <v>698</v>
+        <v>703</v>
       </c>
       <c r="C267" t="s">
-        <v>699</v>
+        <v>704</v>
       </c>
       <c r="D267">
         <v>0</v>
@@ -9335,16 +9416,19 @@
       <c r="G267">
         <v>0</v>
       </c>
+      <c r="H267" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="268" spans="1:8">
       <c r="A268" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
       <c r="B268" t="s">
-        <v>701</v>
+        <v>707</v>
       </c>
       <c r="C268" t="s">
-        <v>702</v>
+        <v>708</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -9356,18 +9440,18 @@
         <v>0.42418181040674502</v>
       </c>
       <c r="G268">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269" spans="1:8">
       <c r="A269" t="s">
-        <v>703</v>
+        <v>709</v>
       </c>
       <c r="B269" t="s">
-        <v>704</v>
+        <v>710</v>
       </c>
       <c r="C269" t="s">
-        <v>705</v>
+        <v>711</v>
       </c>
       <c r="D269">
         <v>0</v>
@@ -9381,16 +9465,19 @@
       <c r="G269">
         <v>0</v>
       </c>
+      <c r="H269" t="s">
+        <v>712</v>
+      </c>
     </row>
     <row r="270" spans="1:8">
       <c r="A270" t="s">
-        <v>706</v>
+        <v>713</v>
       </c>
       <c r="B270" t="s">
-        <v>707</v>
+        <v>714</v>
       </c>
       <c r="C270" t="s">
-        <v>708</v>
+        <v>715</v>
       </c>
       <c r="D270">
         <v>0</v>
@@ -9402,18 +9489,21 @@
         <v>0.84284262931425202</v>
       </c>
       <c r="G270">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H270" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="271" spans="1:8">
       <c r="A271" t="s">
-        <v>709</v>
+        <v>717</v>
       </c>
       <c r="B271" t="s">
-        <v>710</v>
+        <v>718</v>
       </c>
       <c r="C271" t="s">
-        <v>711</v>
+        <v>719</v>
       </c>
       <c r="D271">
         <v>0</v>
@@ -9425,18 +9515,21 @@
         <v>0.66249281383433167</v>
       </c>
       <c r="G271">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H271" t="s">
+        <v>720</v>
       </c>
     </row>
     <row r="272" spans="1:8">
       <c r="A272" t="s">
-        <v>712</v>
+        <v>721</v>
       </c>
       <c r="B272" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="C272" t="s">
-        <v>714</v>
+        <v>723</v>
       </c>
       <c r="D272">
         <v>0</v>
@@ -9450,16 +9543,19 @@
       <c r="G272">
         <v>0</v>
       </c>
-    </row>
-    <row r="273" spans="1:7">
+      <c r="H272" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8">
       <c r="A273" t="s">
-        <v>715</v>
+        <v>725</v>
       </c>
       <c r="B273" t="s">
-        <v>716</v>
+        <v>726</v>
       </c>
       <c r="C273" t="s">
-        <v>717</v>
+        <v>727</v>
       </c>
       <c r="D273">
         <v>0</v>
@@ -9471,18 +9567,21 @@
         <v>0.94038844209558814</v>
       </c>
       <c r="G273">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="274" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H273" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8">
       <c r="A274" t="s">
-        <v>718</v>
+        <v>729</v>
       </c>
       <c r="B274" t="s">
-        <v>719</v>
+        <v>730</v>
       </c>
       <c r="C274" t="s">
-        <v>720</v>
+        <v>731</v>
       </c>
       <c r="D274">
         <v>0</v>
@@ -9494,18 +9593,21 @@
         <v>0.50270270270270279</v>
       </c>
       <c r="G274">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="275" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H274" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8">
       <c r="A275" t="s">
-        <v>721</v>
+        <v>733</v>
       </c>
       <c r="B275" t="s">
-        <v>722</v>
+        <v>734</v>
       </c>
       <c r="C275" t="s">
-        <v>723</v>
+        <v>735</v>
       </c>
       <c r="D275">
         <v>0</v>
@@ -9517,18 +9619,21 @@
         <v>0.3532304111482461</v>
       </c>
       <c r="G275">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="276" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H275" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8">
       <c r="A276" t="s">
-        <v>724</v>
+        <v>737</v>
       </c>
       <c r="B276" t="s">
-        <v>725</v>
+        <v>738</v>
       </c>
       <c r="C276" t="s">
-        <v>726</v>
+        <v>739</v>
       </c>
       <c r="D276">
         <v>0</v>
@@ -9542,16 +9647,19 @@
       <c r="G276">
         <v>0</v>
       </c>
-    </row>
-    <row r="277" spans="1:7">
+      <c r="H276" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8">
       <c r="A277" t="s">
-        <v>727</v>
+        <v>741</v>
       </c>
       <c r="B277" t="s">
-        <v>728</v>
+        <v>742</v>
       </c>
       <c r="C277" t="s">
-        <v>729</v>
+        <v>743</v>
       </c>
       <c r="D277">
         <v>0</v>
@@ -9565,16 +9673,19 @@
       <c r="G277">
         <v>0</v>
       </c>
-    </row>
-    <row r="278" spans="1:7">
+      <c r="H277" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8">
       <c r="A278" t="s">
-        <v>730</v>
+        <v>745</v>
       </c>
       <c r="B278" t="s">
-        <v>731</v>
+        <v>746</v>
       </c>
       <c r="C278" t="s">
-        <v>731</v>
+        <v>746</v>
       </c>
       <c r="D278">
         <v>1</v>
@@ -9589,15 +9700,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:7">
+    <row r="279" spans="1:8">
       <c r="A279" t="s">
-        <v>732</v>
+        <v>747</v>
       </c>
       <c r="B279" t="s">
-        <v>733</v>
+        <v>748</v>
       </c>
       <c r="C279" t="s">
-        <v>734</v>
+        <v>749</v>
       </c>
       <c r="D279">
         <v>0</v>
@@ -9611,16 +9722,19 @@
       <c r="G279">
         <v>0</v>
       </c>
-    </row>
-    <row r="280" spans="1:7">
+      <c r="H279" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8">
       <c r="A280" t="s">
-        <v>735</v>
+        <v>750</v>
       </c>
       <c r="B280" t="s">
-        <v>736</v>
+        <v>751</v>
       </c>
       <c r="C280" t="s">
-        <v>736</v>
+        <v>751</v>
       </c>
       <c r="D280">
         <v>1</v>
@@ -9635,15 +9749,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:7">
+    <row r="281" spans="1:8">
       <c r="A281" t="s">
-        <v>737</v>
+        <v>752</v>
       </c>
       <c r="B281" t="s">
-        <v>738</v>
+        <v>753</v>
       </c>
       <c r="C281" t="s">
-        <v>739</v>
+        <v>754</v>
       </c>
       <c r="D281">
         <v>0</v>
@@ -9655,18 +9769,18 @@
         <v>0.99795199999999995</v>
       </c>
       <c r="G281">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="282" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8">
       <c r="A282" t="s">
-        <v>740</v>
+        <v>755</v>
       </c>
       <c r="B282" t="s">
-        <v>741</v>
+        <v>756</v>
       </c>
       <c r="C282" t="s">
-        <v>741</v>
+        <v>756</v>
       </c>
       <c r="D282">
         <v>1</v>
@@ -9681,15 +9795,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:7">
+    <row r="283" spans="1:8">
       <c r="A283" t="s">
-        <v>742</v>
+        <v>757</v>
       </c>
       <c r="B283" t="s">
-        <v>743</v>
+        <v>758</v>
       </c>
       <c r="C283" t="s">
-        <v>744</v>
+        <v>759</v>
       </c>
       <c r="D283">
         <v>0</v>
@@ -9703,16 +9817,19 @@
       <c r="G283">
         <v>0</v>
       </c>
-    </row>
-    <row r="284" spans="1:7">
+      <c r="H283" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8">
       <c r="A284" t="s">
-        <v>745</v>
+        <v>761</v>
       </c>
       <c r="B284" t="s">
-        <v>746</v>
+        <v>762</v>
       </c>
       <c r="C284" t="s">
-        <v>747</v>
+        <v>763</v>
       </c>
       <c r="D284">
         <v>1</v>
@@ -9727,15 +9844,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:7">
+    <row r="285" spans="1:8">
       <c r="A285" t="s">
-        <v>748</v>
+        <v>764</v>
       </c>
       <c r="B285" t="s">
-        <v>749</v>
+        <v>765</v>
       </c>
       <c r="C285" t="s">
-        <v>749</v>
+        <v>765</v>
       </c>
       <c r="D285">
         <v>1</v>
@@ -9750,15 +9867,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:7">
+    <row r="286" spans="1:8">
       <c r="A286" t="s">
-        <v>750</v>
+        <v>766</v>
       </c>
       <c r="B286" t="s">
-        <v>751</v>
+        <v>767</v>
       </c>
       <c r="C286" t="s">
-        <v>752</v>
+        <v>768</v>
       </c>
       <c r="D286">
         <v>0</v>
@@ -9773,15 +9890,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:7">
+    <row r="287" spans="1:8">
       <c r="A287" t="s">
-        <v>753</v>
+        <v>769</v>
       </c>
       <c r="B287" t="s">
-        <v>754</v>
+        <v>770</v>
       </c>
       <c r="C287" t="s">
-        <v>755</v>
+        <v>771</v>
       </c>
       <c r="D287">
         <v>0</v>
@@ -9796,15 +9913,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:7">
+    <row r="288" spans="1:8">
       <c r="A288" t="s">
-        <v>756</v>
+        <v>772</v>
       </c>
       <c r="B288" t="s">
-        <v>757</v>
+        <v>773</v>
       </c>
       <c r="C288" t="s">
-        <v>758</v>
+        <v>774</v>
       </c>
       <c r="D288">
         <v>0</v>
@@ -9821,13 +9938,13 @@
     </row>
     <row r="289" spans="1:7">
       <c r="A289" t="s">
-        <v>759</v>
+        <v>775</v>
       </c>
       <c r="B289" t="s">
-        <v>760</v>
+        <v>776</v>
       </c>
       <c r="C289" t="s">
-        <v>761</v>
+        <v>777</v>
       </c>
       <c r="D289">
         <v>0</v>
@@ -9844,13 +9961,13 @@
     </row>
     <row r="290" spans="1:7">
       <c r="A290" t="s">
-        <v>762</v>
+        <v>778</v>
       </c>
       <c r="B290" t="s">
-        <v>763</v>
+        <v>779</v>
       </c>
       <c r="C290" t="s">
-        <v>764</v>
+        <v>780</v>
       </c>
       <c r="D290">
         <v>0</v>
@@ -9867,13 +9984,13 @@
     </row>
     <row r="291" spans="1:7">
       <c r="A291" t="s">
-        <v>765</v>
+        <v>781</v>
       </c>
       <c r="B291" t="s">
-        <v>766</v>
+        <v>782</v>
       </c>
       <c r="C291" t="s">
-        <v>767</v>
+        <v>783</v>
       </c>
       <c r="D291">
         <v>0</v>
@@ -9890,13 +10007,13 @@
     </row>
     <row r="292" spans="1:7">
       <c r="A292" t="s">
-        <v>768</v>
+        <v>784</v>
       </c>
       <c r="B292" t="s">
-        <v>769</v>
+        <v>785</v>
       </c>
       <c r="C292" t="s">
-        <v>770</v>
+        <v>786</v>
       </c>
       <c r="D292">
         <v>0</v>
@@ -9913,13 +10030,13 @@
     </row>
     <row r="293" spans="1:7">
       <c r="A293" t="s">
-        <v>771</v>
+        <v>787</v>
       </c>
       <c r="B293" t="s">
-        <v>772</v>
+        <v>788</v>
       </c>
       <c r="C293" t="s">
-        <v>772</v>
+        <v>788</v>
       </c>
       <c r="D293">
         <v>1</v>
@@ -9936,13 +10053,13 @@
     </row>
     <row r="294" spans="1:7">
       <c r="A294" t="s">
-        <v>773</v>
+        <v>789</v>
       </c>
       <c r="B294" t="s">
-        <v>774</v>
+        <v>790</v>
       </c>
       <c r="C294" t="s">
-        <v>775</v>
+        <v>791</v>
       </c>
       <c r="D294">
         <v>0</v>
@@ -9959,13 +10076,13 @@
     </row>
     <row r="295" spans="1:7">
       <c r="A295" t="s">
-        <v>776</v>
+        <v>792</v>
       </c>
       <c r="B295" t="s">
-        <v>777</v>
+        <v>793</v>
       </c>
       <c r="C295" t="s">
-        <v>778</v>
+        <v>794</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -9982,13 +10099,13 @@
     </row>
     <row r="296" spans="1:7">
       <c r="A296" t="s">
-        <v>779</v>
+        <v>795</v>
       </c>
       <c r="B296" t="s">
-        <v>780</v>
+        <v>796</v>
       </c>
       <c r="C296" t="s">
-        <v>781</v>
+        <v>797</v>
       </c>
       <c r="D296">
         <v>0</v>
@@ -10005,13 +10122,13 @@
     </row>
     <row r="297" spans="1:7">
       <c r="A297" t="s">
-        <v>782</v>
+        <v>798</v>
       </c>
       <c r="B297" t="s">
-        <v>783</v>
+        <v>799</v>
       </c>
       <c r="C297" t="s">
-        <v>784</v>
+        <v>800</v>
       </c>
       <c r="D297">
         <v>0</v>
@@ -10028,13 +10145,13 @@
     </row>
     <row r="298" spans="1:7">
       <c r="A298" t="s">
-        <v>785</v>
+        <v>801</v>
       </c>
       <c r="B298" t="s">
-        <v>786</v>
+        <v>802</v>
       </c>
       <c r="C298" t="s">
-        <v>787</v>
+        <v>803</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -10051,13 +10168,13 @@
     </row>
     <row r="299" spans="1:7">
       <c r="A299" t="s">
-        <v>788</v>
+        <v>804</v>
       </c>
       <c r="B299" t="s">
-        <v>789</v>
+        <v>805</v>
       </c>
       <c r="C299" t="s">
-        <v>789</v>
+        <v>805</v>
       </c>
       <c r="D299">
         <v>1</v>
@@ -10074,13 +10191,13 @@
     </row>
     <row r="300" spans="1:7">
       <c r="A300" t="s">
-        <v>790</v>
+        <v>806</v>
       </c>
       <c r="B300" t="s">
-        <v>791</v>
+        <v>807</v>
       </c>
       <c r="C300" t="s">
-        <v>791</v>
+        <v>807</v>
       </c>
       <c r="D300">
         <v>1</v>
@@ -10097,13 +10214,13 @@
     </row>
     <row r="301" spans="1:7">
       <c r="A301" t="s">
-        <v>792</v>
+        <v>808</v>
       </c>
       <c r="B301" t="s">
-        <v>793</v>
+        <v>809</v>
       </c>
       <c r="C301" t="s">
-        <v>794</v>
+        <v>810</v>
       </c>
       <c r="D301">
         <v>0</v>
@@ -10120,13 +10237,13 @@
     </row>
     <row r="302" spans="1:7">
       <c r="A302" t="s">
-        <v>795</v>
+        <v>811</v>
       </c>
       <c r="B302" t="s">
-        <v>796</v>
+        <v>812</v>
       </c>
       <c r="C302" t="s">
-        <v>797</v>
+        <v>813</v>
       </c>
       <c r="D302">
         <v>0</v>
@@ -10143,13 +10260,13 @@
     </row>
     <row r="303" spans="1:7">
       <c r="A303" t="s">
-        <v>798</v>
+        <v>814</v>
       </c>
       <c r="B303" t="s">
-        <v>799</v>
+        <v>815</v>
       </c>
       <c r="C303" t="s">
-        <v>800</v>
+        <v>816</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -10166,13 +10283,13 @@
     </row>
     <row r="304" spans="1:7">
       <c r="A304" t="s">
-        <v>801</v>
+        <v>817</v>
       </c>
       <c r="B304" t="s">
-        <v>802</v>
+        <v>818</v>
       </c>
       <c r="C304" t="s">
-        <v>803</v>
+        <v>819</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -10189,13 +10306,13 @@
     </row>
     <row r="305" spans="1:7">
       <c r="A305" t="s">
-        <v>804</v>
+        <v>820</v>
       </c>
       <c r="B305" t="s">
-        <v>805</v>
+        <v>821</v>
       </c>
       <c r="C305" t="s">
-        <v>806</v>
+        <v>822</v>
       </c>
       <c r="D305">
         <v>0</v>
@@ -10212,13 +10329,13 @@
     </row>
     <row r="306" spans="1:7">
       <c r="A306" t="s">
-        <v>807</v>
+        <v>823</v>
       </c>
       <c r="B306" t="s">
-        <v>808</v>
+        <v>824</v>
       </c>
       <c r="C306" t="s">
-        <v>809</v>
+        <v>825</v>
       </c>
       <c r="D306">
         <v>0</v>
@@ -10235,13 +10352,13 @@
     </row>
     <row r="307" spans="1:7">
       <c r="A307" t="s">
-        <v>810</v>
+        <v>826</v>
       </c>
       <c r="B307" t="s">
-        <v>811</v>
+        <v>827</v>
       </c>
       <c r="C307" t="s">
-        <v>812</v>
+        <v>828</v>
       </c>
       <c r="D307">
         <v>0</v>
@@ -10258,13 +10375,13 @@
     </row>
     <row r="308" spans="1:7">
       <c r="A308" t="s">
-        <v>813</v>
+        <v>829</v>
       </c>
       <c r="B308" t="s">
-        <v>814</v>
+        <v>830</v>
       </c>
       <c r="C308" t="s">
-        <v>815</v>
+        <v>831</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -10281,13 +10398,13 @@
     </row>
     <row r="309" spans="1:7">
       <c r="A309" t="s">
-        <v>816</v>
+        <v>832</v>
       </c>
       <c r="B309" t="s">
-        <v>817</v>
+        <v>833</v>
       </c>
       <c r="C309" t="s">
-        <v>818</v>
+        <v>834</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -10304,13 +10421,13 @@
     </row>
     <row r="310" spans="1:7">
       <c r="A310" t="s">
-        <v>819</v>
+        <v>835</v>
       </c>
       <c r="B310" t="s">
-        <v>820</v>
+        <v>836</v>
       </c>
       <c r="C310" t="s">
-        <v>820</v>
+        <v>836</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -10327,13 +10444,13 @@
     </row>
     <row r="311" spans="1:7">
       <c r="A311" t="s">
-        <v>821</v>
+        <v>837</v>
       </c>
       <c r="B311" t="s">
-        <v>822</v>
+        <v>838</v>
       </c>
       <c r="C311" t="s">
-        <v>822</v>
+        <v>838</v>
       </c>
       <c r="D311">
         <v>1</v>
@@ -10350,13 +10467,13 @@
     </row>
     <row r="312" spans="1:7">
       <c r="A312" t="s">
-        <v>823</v>
+        <v>839</v>
       </c>
       <c r="B312" t="s">
-        <v>824</v>
+        <v>840</v>
       </c>
       <c r="C312" t="s">
-        <v>825</v>
+        <v>841</v>
       </c>
       <c r="D312">
         <v>0</v>
@@ -10373,13 +10490,13 @@
     </row>
     <row r="313" spans="1:7">
       <c r="A313" t="s">
-        <v>826</v>
+        <v>842</v>
       </c>
       <c r="B313" t="s">
-        <v>827</v>
+        <v>843</v>
       </c>
       <c r="C313" t="s">
-        <v>828</v>
+        <v>844</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -10396,13 +10513,13 @@
     </row>
     <row r="314" spans="1:7">
       <c r="A314" t="s">
-        <v>829</v>
+        <v>845</v>
       </c>
       <c r="B314" t="s">
-        <v>830</v>
+        <v>846</v>
       </c>
       <c r="C314" t="s">
-        <v>831</v>
+        <v>847</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -10419,13 +10536,13 @@
     </row>
     <row r="315" spans="1:7">
       <c r="A315" t="s">
-        <v>832</v>
+        <v>848</v>
       </c>
       <c r="B315" t="s">
-        <v>833</v>
+        <v>849</v>
       </c>
       <c r="C315" t="s">
-        <v>834</v>
+        <v>850</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -10442,13 +10559,13 @@
     </row>
     <row r="316" spans="1:7">
       <c r="A316" t="s">
-        <v>835</v>
+        <v>851</v>
       </c>
       <c r="B316" t="s">
-        <v>836</v>
+        <v>852</v>
       </c>
       <c r="C316" t="s">
-        <v>837</v>
+        <v>853</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -10465,13 +10582,13 @@
     </row>
     <row r="317" spans="1:7">
       <c r="A317" t="s">
-        <v>838</v>
+        <v>854</v>
       </c>
       <c r="B317" t="s">
-        <v>839</v>
+        <v>855</v>
       </c>
       <c r="C317" t="s">
-        <v>840</v>
+        <v>856</v>
       </c>
       <c r="D317">
         <v>0</v>
@@ -10488,13 +10605,13 @@
     </row>
     <row r="318" spans="1:7">
       <c r="A318" t="s">
-        <v>841</v>
+        <v>857</v>
       </c>
       <c r="B318" t="s">
-        <v>842</v>
+        <v>858</v>
       </c>
       <c r="C318" t="s">
-        <v>843</v>
+        <v>859</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -10511,13 +10628,13 @@
     </row>
     <row r="319" spans="1:7">
       <c r="A319" t="s">
-        <v>844</v>
+        <v>860</v>
       </c>
       <c r="B319" t="s">
-        <v>845</v>
+        <v>861</v>
       </c>
       <c r="C319" t="s">
-        <v>846</v>
+        <v>862</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -10534,13 +10651,13 @@
     </row>
     <row r="320" spans="1:7">
       <c r="A320" t="s">
-        <v>847</v>
+        <v>863</v>
       </c>
       <c r="B320" t="s">
-        <v>848</v>
+        <v>864</v>
       </c>
       <c r="C320" t="s">
-        <v>849</v>
+        <v>865</v>
       </c>
       <c r="D320">
         <v>0</v>
@@ -10557,13 +10674,13 @@
     </row>
     <row r="321" spans="1:7">
       <c r="A321" t="s">
-        <v>850</v>
+        <v>866</v>
       </c>
       <c r="B321" t="s">
-        <v>851</v>
+        <v>867</v>
       </c>
       <c r="C321" t="s">
-        <v>851</v>
+        <v>867</v>
       </c>
       <c r="D321">
         <v>1</v>
@@ -10580,13 +10697,13 @@
     </row>
     <row r="322" spans="1:7">
       <c r="A322" t="s">
-        <v>852</v>
+        <v>868</v>
       </c>
       <c r="B322" t="s">
-        <v>853</v>
+        <v>869</v>
       </c>
       <c r="C322" t="s">
-        <v>853</v>
+        <v>869</v>
       </c>
       <c r="D322">
         <v>1</v>
@@ -10603,13 +10720,13 @@
     </row>
     <row r="323" spans="1:7">
       <c r="A323" t="s">
-        <v>854</v>
+        <v>870</v>
       </c>
       <c r="B323" t="s">
-        <v>855</v>
+        <v>871</v>
       </c>
       <c r="C323" t="s">
-        <v>855</v>
+        <v>871</v>
       </c>
       <c r="D323">
         <v>1</v>
@@ -10626,13 +10743,13 @@
     </row>
     <row r="324" spans="1:7">
       <c r="A324" t="s">
-        <v>856</v>
+        <v>872</v>
       </c>
       <c r="B324" t="s">
-        <v>857</v>
+        <v>873</v>
       </c>
       <c r="C324" t="s">
-        <v>858</v>
+        <v>874</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -10649,13 +10766,13 @@
     </row>
     <row r="325" spans="1:7">
       <c r="A325" t="s">
-        <v>859</v>
+        <v>875</v>
       </c>
       <c r="B325" t="s">
-        <v>860</v>
+        <v>876</v>
       </c>
       <c r="C325" t="s">
-        <v>861</v>
+        <v>877</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -10672,13 +10789,13 @@
     </row>
     <row r="326" spans="1:7">
       <c r="A326" t="s">
-        <v>862</v>
+        <v>878</v>
       </c>
       <c r="B326" t="s">
-        <v>863</v>
+        <v>879</v>
       </c>
       <c r="C326" t="s">
-        <v>863</v>
+        <v>879</v>
       </c>
       <c r="D326">
         <v>1</v>
@@ -10695,13 +10812,13 @@
     </row>
     <row r="327" spans="1:7">
       <c r="A327" t="s">
-        <v>864</v>
+        <v>880</v>
       </c>
       <c r="B327" t="s">
-        <v>865</v>
+        <v>881</v>
       </c>
       <c r="C327" t="s">
-        <v>865</v>
+        <v>881</v>
       </c>
       <c r="D327">
         <v>1</v>

</xml_diff>

<commit_message>
Termine analisi CodeGen e statistiche finali
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/AnalisiCodeGen.xlsx
+++ b/HE/W_in_progress/AnalisiCodeGen.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28209"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{340FD3F4-FACB-4164-9B8A-66C725823AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8546F6C5-CD0D-43DB-89C5-60D4910FC355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="896">
   <si>
     <t>IN</t>
   </si>
@@ -2622,6 +2622,9 @@
     <t>signal output_val : std_logic; if bar(21 downto 14) = x"2B" then ; end if;; if bar(21 downto 14) = x"2B" then ; end if;</t>
   </si>
   <si>
+    <t>u1 non lo inizializza</t>
+  </si>
+  <si>
     <t>Define and declare multiple signals of type std_logic: en_tmp, req_tmp, ack_tmp, write_tmp; i_ldac_cnt is an integer signal ranging from 0 to 4.</t>
   </si>
   <si>
@@ -2640,6 +2643,9 @@
     <t>if ghi(16 downto 9) = x"77" then ; end if; case w is when "U" =&gt; w := "X"; when "X" =&gt; ; when "0" =&gt; w := w2; when "+" | "-" =&gt; if w2 = '0' then w := w1; end if; end case;</t>
   </si>
   <si>
+    <t>Non spiaccicati ma sintatticamente simili</t>
+  </si>
+  <si>
     <t>ROM_selector_onboard is an entity with clock_in as input std_logic signal, reset_in as input std_logic signal, addr_strobe_in as input std_logic signal, anodes_out as output std_logic_vector signal of 8 bit, cathodes_out as output std_logic_vector signal of 8 bit; temp_stop_cu ia s std_logic signal; define a signal of type std_logic initialized to 0 and called TbClockA</t>
   </si>
   <si>
@@ -2649,6 +2655,9 @@
     <t>entity ROM_selector_onboard is port (clock_in : in STD_LOGIC; reset_in : in STD_LOGIC; addr_strobe_in : in STD_LOGIC; anodes_out : out STD_LOGIC_VECTOR(7 downto 0); cathodes_out : out STD_LOGIC_VECTOR(7 downto 0)); end ROM_selector_onboard; signal temp_stop_cu: std_logic;; signal TbClockA : std_logic;</t>
   </si>
   <si>
+    <t>Non a ciò che gli ho richiesto</t>
+  </si>
+  <si>
     <t>Define an entity named ripple_carry with input signals X and Y each of size 8 bits, s_in as a single bit input signal, c_out as a single bit output signal, and Z as an output std_logic_vector of size 8 bits; using the selected signal assignment, the signal c.a_request.be is set to c.sys_master_ctrl_out.be when the signal c.b_request_complete is equal to '1', r.b_request.be when the signal c.b_request_complete is equal to '0', otherwise 'X'; define the ieee standard library</t>
   </si>
   <si>
@@ -2676,6 +2685,9 @@
     <t>clk2xgen: if (clk2xen /= 0) generate clkena(1 downto 0) &lt;= "11"; end generate; signal round_key_temp: std_logic_vector(63 downto 0);; component sbox is port(data_in: in std_logic_vector(3 downto 0); data_out: out std_logic_vector(3 downto 0)); end component;</t>
   </si>
   <si>
+    <t xml:space="preserve">identiche,  a parte la definizione di sbox che però è generica </t>
+  </si>
+  <si>
     <t>t_stb is a signal of type std_logic; concatenate two 18-bit slices from reg_key_in and two 61-bit slices from reg_key_in, store the result in key_temp1</t>
   </si>
   <si>
@@ -2683,6 +2695,9 @@
   </si>
   <si>
     <t>signal_t_stb : std_logic; reg_key_in( 18 downto 0 ) &lt;= reg_key_in( 18 downto 0 ) &amp; reg_key_in( 79 downto 19 ); reg_key_in( 79 downto 19 ) &lt;= reg_key_in( 18 downto 0 ) &amp; reg_key_in( 79 downto 19 );</t>
+  </si>
+  <si>
+    <t>Sbaliata l'assegnazione</t>
   </si>
   <si>
     <t>set signal result_sig as the XOR of input_x and input_y; i_sck_cpy is a signal of type std_logic; pl is an instance of perm_layer component with the signals data_out_temp2, data_out</t>
@@ -3120,7 +3135,7 @@
   <dimension ref="A1:H327"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
-      <selection activeCell="K311" sqref="K311"/>
+      <selection activeCell="E330" sqref="E330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10479,7 +10494,7 @@
         <v>0.99995890523547304</v>
       </c>
       <c r="G309">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="310" spans="1:8">
@@ -10550,16 +10565,19 @@
       <c r="G312">
         <v>0</v>
       </c>
+      <c r="H312" t="s">
+        <v>851</v>
+      </c>
     </row>
     <row r="313" spans="1:8">
       <c r="A313" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B313" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="C313" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -10571,18 +10589,18 @@
         <v>0.99993750000000003</v>
       </c>
       <c r="G313">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="314" spans="1:8">
       <c r="A314" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B314" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C314" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -10594,18 +10612,21 @@
         <v>0.74591538743156838</v>
       </c>
       <c r="G314">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H314" t="s">
+        <v>858</v>
       </c>
     </row>
     <row r="315" spans="1:8">
       <c r="A315" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="B315" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="C315" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -10619,16 +10640,19 @@
       <c r="G315">
         <v>0</v>
       </c>
+      <c r="H315" t="s">
+        <v>862</v>
+      </c>
     </row>
     <row r="316" spans="1:8">
       <c r="A316" t="s">
-        <v>860</v>
+        <v>863</v>
       </c>
       <c r="B316" t="s">
-        <v>861</v>
+        <v>864</v>
       </c>
       <c r="C316" t="s">
-        <v>862</v>
+        <v>865</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -10640,18 +10664,18 @@
         <v>0.94454085945451716</v>
       </c>
       <c r="G316">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317" spans="1:8">
       <c r="A317" t="s">
-        <v>863</v>
+        <v>866</v>
       </c>
       <c r="B317" t="s">
-        <v>864</v>
+        <v>867</v>
       </c>
       <c r="C317" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="D317">
         <v>0</v>
@@ -10665,16 +10689,19 @@
       <c r="G317">
         <v>0</v>
       </c>
+      <c r="H317" t="s">
+        <v>581</v>
+      </c>
     </row>
     <row r="318" spans="1:8">
       <c r="A318" t="s">
-        <v>866</v>
+        <v>869</v>
       </c>
       <c r="B318" t="s">
-        <v>867</v>
+        <v>870</v>
       </c>
       <c r="C318" t="s">
-        <v>868</v>
+        <v>871</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -10686,18 +10713,21 @@
         <v>0.87722761852115083</v>
       </c>
       <c r="G318">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H318" t="s">
+        <v>872</v>
       </c>
     </row>
     <row r="319" spans="1:8">
       <c r="A319" t="s">
-        <v>869</v>
+        <v>873</v>
       </c>
       <c r="B319" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
       <c r="C319" t="s">
-        <v>871</v>
+        <v>875</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -10711,16 +10741,19 @@
       <c r="G319">
         <v>0</v>
       </c>
+      <c r="H319" t="s">
+        <v>876</v>
+      </c>
     </row>
     <row r="320" spans="1:8">
       <c r="A320" t="s">
-        <v>872</v>
+        <v>877</v>
       </c>
       <c r="B320" t="s">
-        <v>873</v>
+        <v>878</v>
       </c>
       <c r="C320" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="D320">
         <v>0</v>
@@ -10732,18 +10765,18 @@
         <v>0.98943985307621674</v>
       </c>
       <c r="G320">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="321" spans="1:7">
       <c r="A321" t="s">
-        <v>875</v>
+        <v>880</v>
       </c>
       <c r="B321" t="s">
-        <v>876</v>
+        <v>881</v>
       </c>
       <c r="C321" t="s">
-        <v>876</v>
+        <v>881</v>
       </c>
       <c r="D321">
         <v>1</v>
@@ -10760,13 +10793,13 @@
     </row>
     <row r="322" spans="1:7">
       <c r="A322" t="s">
-        <v>877</v>
+        <v>882</v>
       </c>
       <c r="B322" t="s">
-        <v>878</v>
+        <v>883</v>
       </c>
       <c r="C322" t="s">
-        <v>878</v>
+        <v>883</v>
       </c>
       <c r="D322">
         <v>1</v>
@@ -10783,13 +10816,13 @@
     </row>
     <row r="323" spans="1:7">
       <c r="A323" t="s">
-        <v>879</v>
+        <v>884</v>
       </c>
       <c r="B323" t="s">
-        <v>880</v>
+        <v>885</v>
       </c>
       <c r="C323" t="s">
-        <v>880</v>
+        <v>885</v>
       </c>
       <c r="D323">
         <v>1</v>
@@ -10806,13 +10839,13 @@
     </row>
     <row r="324" spans="1:7">
       <c r="A324" t="s">
-        <v>881</v>
+        <v>886</v>
       </c>
       <c r="B324" t="s">
-        <v>882</v>
+        <v>887</v>
       </c>
       <c r="C324" t="s">
-        <v>883</v>
+        <v>888</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -10824,18 +10857,18 @@
         <v>0.96995416256349587</v>
       </c>
       <c r="G324">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="325" spans="1:7">
       <c r="A325" t="s">
-        <v>884</v>
+        <v>889</v>
       </c>
       <c r="B325" t="s">
-        <v>885</v>
+        <v>890</v>
       </c>
       <c r="C325" t="s">
-        <v>886</v>
+        <v>891</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -10847,18 +10880,18 @@
         <v>0.9999968246710359</v>
       </c>
       <c r="G325">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="326" spans="1:7">
       <c r="A326" t="s">
-        <v>887</v>
+        <v>892</v>
       </c>
       <c r="B326" t="s">
-        <v>888</v>
+        <v>893</v>
       </c>
       <c r="C326" t="s">
-        <v>888</v>
+        <v>893</v>
       </c>
       <c r="D326">
         <v>1</v>
@@ -10875,13 +10908,13 @@
     </row>
     <row r="327" spans="1:7">
       <c r="A327" t="s">
-        <v>889</v>
+        <v>894</v>
       </c>
       <c r="B327" t="s">
-        <v>890</v>
+        <v>895</v>
       </c>
       <c r="C327" t="s">
-        <v>890</v>
+        <v>895</v>
       </c>
       <c r="D327">
         <v>1</v>

</xml_diff>